<commit_message>
Updated: po 14. 12. 2020
</commit_message>
<xml_diff>
--- a/OpenData_Slovakia_Covid_DailyStats.xlsx
+++ b/OpenData_Slovakia_Covid_DailyStats.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I281"/>
+  <dimension ref="A1:I284"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -6979,7 +6979,7 @@
         <v>930</v>
       </c>
       <c r="H273">
-        <v>25974</v>
+        <v>25977</v>
       </c>
       <c r="I273">
         <v>1301</v>
@@ -7153,7 +7153,7 @@
         <v>1084</v>
       </c>
       <c r="H279">
-        <v>42215</v>
+        <v>42220</v>
       </c>
       <c r="I279">
         <v>2946</v>
@@ -7182,10 +7182,10 @@
         <v>1104</v>
       </c>
       <c r="H280">
-        <v>32253</v>
+        <v>32670</v>
       </c>
       <c r="I280">
-        <v>2079</v>
+        <v>2130</v>
       </c>
     </row>
     <row r="281">
@@ -7211,10 +7211,97 @@
         <v>1122</v>
       </c>
       <c r="H281">
-        <v>39160</v>
+        <v>41465</v>
       </c>
       <c r="I281">
-        <v>2810</v>
+        <v>2940</v>
+      </c>
+    </row>
+    <row r="282">
+      <c r="A282" s="2">
+        <v>44176</v>
+      </c>
+      <c r="B282">
+        <v>130794</v>
+      </c>
+      <c r="C282">
+        <v>95416</v>
+      </c>
+      <c r="D282">
+        <v>34230</v>
+      </c>
+      <c r="E282">
+        <v>17956</v>
+      </c>
+      <c r="F282">
+        <v>3707</v>
+      </c>
+      <c r="G282">
+        <v>1148</v>
+      </c>
+      <c r="H282">
+        <v>42243</v>
+      </c>
+      <c r="I282">
+        <v>2545</v>
+      </c>
+    </row>
+    <row r="283">
+      <c r="A283" s="2">
+        <v>44177</v>
+      </c>
+      <c r="B283">
+        <v>132984</v>
+      </c>
+      <c r="C283">
+        <v>97068</v>
+      </c>
+      <c r="D283">
+        <v>34741</v>
+      </c>
+      <c r="E283">
+        <v>9991</v>
+      </c>
+      <c r="F283">
+        <v>2190</v>
+      </c>
+      <c r="G283">
+        <v>1175</v>
+      </c>
+      <c r="H283">
+        <v>15304</v>
+      </c>
+      <c r="I283">
+        <v>911</v>
+      </c>
+    </row>
+    <row r="284">
+      <c r="A284" s="2">
+        <v>44178</v>
+      </c>
+      <c r="B284">
+        <v>133489</v>
+      </c>
+      <c r="C284">
+        <v>98585</v>
+      </c>
+      <c r="D284">
+        <v>33699</v>
+      </c>
+      <c r="E284">
+        <v>2899</v>
+      </c>
+      <c r="F284">
+        <v>505</v>
+      </c>
+      <c r="G284">
+        <v>1205</v>
+      </c>
+      <c r="H284">
+        <v>1509</v>
+      </c>
+      <c r="I284">
+        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated: st 16. 12. 2020
</commit_message>
<xml_diff>
--- a/OpenData_Slovakia_Covid_DailyStats.xlsx
+++ b/OpenData_Slovakia_Covid_DailyStats.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I285"/>
+  <dimension ref="A1:I286"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -5447,6 +5447,12 @@
       <c r="G220">
         <v>61</v>
       </c>
+      <c r="H220">
+        <v>0</v>
+      </c>
+      <c r="I220">
+        <v>0</v>
+      </c>
     </row>
     <row r="221">
       <c r="A221" s="2">
@@ -5471,10 +5477,10 @@
         <v>61</v>
       </c>
       <c r="H221">
-        <v>0</v>
+        <v>525</v>
       </c>
       <c r="I221">
-        <v>0</v>
+        <v>40</v>
       </c>
     </row>
     <row r="222">
@@ -5500,10 +5506,10 @@
         <v>61</v>
       </c>
       <c r="H222">
-        <v>525</v>
+        <v>1155</v>
       </c>
       <c r="I222">
-        <v>40</v>
+        <v>84</v>
       </c>
     </row>
     <row r="223">
@@ -5529,10 +5535,10 @@
         <v>66</v>
       </c>
       <c r="H223">
-        <v>1155</v>
+        <v>929</v>
       </c>
       <c r="I223">
-        <v>84</v>
+        <v>31</v>
       </c>
     </row>
     <row r="224">
@@ -5558,10 +5564,10 @@
         <v>71</v>
       </c>
       <c r="H224">
-        <v>929</v>
+        <v>372</v>
       </c>
       <c r="I224">
-        <v>31</v>
+        <v>36</v>
       </c>
     </row>
     <row r="225">
@@ -5587,10 +5593,10 @@
         <v>71</v>
       </c>
       <c r="H225">
-        <v>372</v>
+        <v>320</v>
       </c>
       <c r="I225">
-        <v>36</v>
+        <v>27</v>
       </c>
     </row>
     <row r="226">
@@ -5616,10 +5622,10 @@
         <v>82</v>
       </c>
       <c r="H226">
-        <v>320</v>
+        <v>0</v>
       </c>
       <c r="I226">
-        <v>27</v>
+        <v>0</v>
       </c>
     </row>
     <row r="227">
@@ -5645,7 +5651,7 @@
         <v>88</v>
       </c>
       <c r="H227">
-        <v>0</v>
+        <v>92</v>
       </c>
       <c r="I227">
         <v>0</v>
@@ -5674,10 +5680,10 @@
         <v>92</v>
       </c>
       <c r="H228">
-        <v>92</v>
+        <v>792</v>
       </c>
       <c r="I228">
-        <v>0</v>
+        <v>69</v>
       </c>
     </row>
     <row r="229">
@@ -5703,10 +5709,10 @@
         <v>98</v>
       </c>
       <c r="H229">
-        <v>792</v>
+        <v>613</v>
       </c>
       <c r="I229">
-        <v>69</v>
+        <v>38</v>
       </c>
     </row>
     <row r="230">
@@ -5732,10 +5738,10 @@
         <v>98</v>
       </c>
       <c r="H230">
-        <v>613</v>
+        <v>954</v>
       </c>
       <c r="I230">
-        <v>38</v>
+        <v>48</v>
       </c>
     </row>
     <row r="231">
@@ -5761,10 +5767,10 @@
         <v>115</v>
       </c>
       <c r="H231">
-        <v>954</v>
+        <v>2136</v>
       </c>
       <c r="I231">
-        <v>48</v>
+        <v>141</v>
       </c>
     </row>
     <row r="232">
@@ -5790,10 +5796,10 @@
         <v>134</v>
       </c>
       <c r="H232">
-        <v>2136</v>
+        <v>2161</v>
       </c>
       <c r="I232">
-        <v>141</v>
+        <v>119</v>
       </c>
     </row>
     <row r="233">
@@ -5819,10 +5825,10 @@
         <v>159</v>
       </c>
       <c r="H233">
-        <v>2161</v>
+        <v>1194</v>
       </c>
       <c r="I233">
-        <v>119</v>
+        <v>65</v>
       </c>
     </row>
     <row r="234">
@@ -5848,10 +5854,10 @@
         <v>159</v>
       </c>
       <c r="H234">
-        <v>1194</v>
+        <v>729</v>
       </c>
       <c r="I234">
-        <v>65</v>
+        <v>40</v>
       </c>
     </row>
     <row r="235">
@@ -5877,10 +5883,10 @@
         <v>165</v>
       </c>
       <c r="H235">
-        <v>729</v>
+        <v>2161</v>
       </c>
       <c r="I235">
-        <v>40</v>
+        <v>231</v>
       </c>
     </row>
     <row r="236">
@@ -5906,10 +5912,10 @@
         <v>176</v>
       </c>
       <c r="H236">
-        <v>2161</v>
+        <v>3036</v>
       </c>
       <c r="I236">
-        <v>231</v>
+        <v>234</v>
       </c>
     </row>
     <row r="237">
@@ -5935,10 +5941,10 @@
         <v>184</v>
       </c>
       <c r="H237">
-        <v>3036</v>
+        <v>2415</v>
       </c>
       <c r="I237">
-        <v>234</v>
+        <v>225</v>
       </c>
     </row>
     <row r="238">
@@ -5964,10 +5970,10 @@
         <v>200</v>
       </c>
       <c r="H238">
-        <v>2415</v>
+        <v>6149</v>
       </c>
       <c r="I238">
-        <v>225</v>
+        <v>239</v>
       </c>
     </row>
     <row r="239">
@@ -5993,10 +5999,10 @@
         <v>212</v>
       </c>
       <c r="H239">
-        <v>6149</v>
+        <v>41133</v>
       </c>
       <c r="I239">
-        <v>239</v>
+        <v>471</v>
       </c>
     </row>
     <row r="240">
@@ -6022,10 +6028,10 @@
         <v>219</v>
       </c>
       <c r="H240">
-        <v>41133</v>
+        <v>89674</v>
       </c>
       <c r="I240">
-        <v>471</v>
+        <v>975</v>
       </c>
     </row>
     <row r="241">
@@ -6051,10 +6057,10 @@
         <v>219</v>
       </c>
       <c r="H241">
-        <v>89674</v>
+        <v>30176</v>
       </c>
       <c r="I241">
-        <v>975</v>
+        <v>376</v>
       </c>
     </row>
     <row r="242">
@@ -6080,10 +6086,10 @@
         <v>219</v>
       </c>
       <c r="H242">
-        <v>30176</v>
+        <v>26701</v>
       </c>
       <c r="I242">
-        <v>376</v>
+        <v>1331</v>
       </c>
     </row>
     <row r="243">
@@ -6109,10 +6115,10 @@
         <v>235</v>
       </c>
       <c r="H243">
-        <v>26701</v>
+        <v>5279</v>
       </c>
       <c r="I243">
-        <v>1331</v>
+        <v>98</v>
       </c>
     </row>
     <row r="244">
@@ -6138,10 +6144,10 @@
         <v>261</v>
       </c>
       <c r="H244">
-        <v>5279</v>
+        <v>3592</v>
       </c>
       <c r="I244">
-        <v>98</v>
+        <v>82</v>
       </c>
     </row>
     <row r="245">
@@ -6167,10 +6173,10 @@
         <v>286</v>
       </c>
       <c r="H245">
-        <v>3592</v>
+        <v>2115</v>
       </c>
       <c r="I245">
-        <v>82</v>
+        <v>140</v>
       </c>
     </row>
     <row r="246">
@@ -6196,10 +6202,10 @@
         <v>317</v>
       </c>
       <c r="H246">
-        <v>2115</v>
+        <v>34523</v>
       </c>
       <c r="I246">
-        <v>140</v>
+        <v>327</v>
       </c>
     </row>
     <row r="247">
@@ -6225,10 +6231,10 @@
         <v>351</v>
       </c>
       <c r="H247">
-        <v>34523</v>
+        <v>45190</v>
       </c>
       <c r="I247">
-        <v>327</v>
+        <v>439</v>
       </c>
     </row>
     <row r="248">
@@ -6254,10 +6260,10 @@
         <v>351</v>
       </c>
       <c r="H248">
-        <v>45190</v>
+        <v>12172</v>
       </c>
       <c r="I248">
-        <v>439</v>
+        <v>143</v>
       </c>
     </row>
     <row r="249">
@@ -6283,10 +6289,10 @@
         <v>366</v>
       </c>
       <c r="H249">
-        <v>12172</v>
+        <v>17651</v>
       </c>
       <c r="I249">
-        <v>143</v>
+        <v>1154</v>
       </c>
     </row>
     <row r="250">
@@ -6312,10 +6318,10 @@
         <v>390</v>
       </c>
       <c r="H250">
-        <v>17651</v>
+        <v>6492</v>
       </c>
       <c r="I250">
-        <v>1154</v>
+        <v>140</v>
       </c>
     </row>
     <row r="251">
@@ -6341,10 +6347,10 @@
         <v>414</v>
       </c>
       <c r="H251">
-        <v>6492</v>
+        <v>4620</v>
       </c>
       <c r="I251">
-        <v>140</v>
+        <v>101</v>
       </c>
     </row>
     <row r="252">
@@ -6370,10 +6376,10 @@
         <v>464</v>
       </c>
       <c r="H252">
-        <v>4620</v>
+        <v>5606</v>
       </c>
       <c r="I252">
-        <v>101</v>
+        <v>173</v>
       </c>
     </row>
     <row r="253">
@@ -6399,10 +6405,10 @@
         <v>491</v>
       </c>
       <c r="H253">
-        <v>5606</v>
+        <v>6144</v>
       </c>
       <c r="I253">
-        <v>173</v>
+        <v>158</v>
       </c>
     </row>
     <row r="254">
@@ -6428,10 +6434,10 @@
         <v>510</v>
       </c>
       <c r="H254">
-        <v>6144</v>
+        <v>5452</v>
       </c>
       <c r="I254">
-        <v>158</v>
+        <v>99</v>
       </c>
     </row>
     <row r="255">
@@ -6457,10 +6463,10 @@
         <v>510</v>
       </c>
       <c r="H255">
-        <v>5452</v>
+        <v>1242</v>
       </c>
       <c r="I255">
-        <v>99</v>
+        <v>33</v>
       </c>
     </row>
     <row r="256">
@@ -6486,10 +6492,10 @@
         <v>526</v>
       </c>
       <c r="H256">
-        <v>1242</v>
+        <v>5258</v>
       </c>
       <c r="I256">
-        <v>33</v>
+        <v>275</v>
       </c>
     </row>
     <row r="257">
@@ -6515,10 +6521,10 @@
         <v>557</v>
       </c>
       <c r="H257">
-        <v>5258</v>
+        <v>3874</v>
       </c>
       <c r="I257">
-        <v>275</v>
+        <v>220</v>
       </c>
     </row>
     <row r="258">
@@ -6544,10 +6550,10 @@
         <v>579</v>
       </c>
       <c r="H258">
-        <v>3874</v>
+        <v>6114</v>
       </c>
       <c r="I258">
-        <v>220</v>
+        <v>423</v>
       </c>
     </row>
     <row r="259">
@@ -6573,10 +6579,10 @@
         <v>579</v>
       </c>
       <c r="H259">
-        <v>6114</v>
+        <v>11540</v>
       </c>
       <c r="I259">
-        <v>423</v>
+        <v>750</v>
       </c>
     </row>
     <row r="260">
@@ -6602,10 +6608,10 @@
         <v>614</v>
       </c>
       <c r="H260">
-        <v>11540</v>
+        <v>17458</v>
       </c>
       <c r="I260">
-        <v>750</v>
+        <v>597</v>
       </c>
     </row>
     <row r="261">
@@ -6631,10 +6637,10 @@
         <v>644</v>
       </c>
       <c r="H261">
-        <v>17458</v>
+        <v>9226</v>
       </c>
       <c r="I261">
-        <v>597</v>
+        <v>317</v>
       </c>
     </row>
     <row r="262">
@@ -6660,10 +6666,10 @@
         <v>671</v>
       </c>
       <c r="H262">
-        <v>9226</v>
+        <v>1701</v>
       </c>
       <c r="I262">
-        <v>317</v>
+        <v>57</v>
       </c>
     </row>
     <row r="263">
@@ -6689,10 +6695,10 @@
         <v>693</v>
       </c>
       <c r="H263">
-        <v>1701</v>
+        <v>42064</v>
       </c>
       <c r="I263">
-        <v>57</v>
+        <v>860</v>
       </c>
     </row>
     <row r="264">
@@ -6718,10 +6724,10 @@
         <v>709</v>
       </c>
       <c r="H264">
-        <v>42064</v>
+        <v>17221</v>
       </c>
       <c r="I264">
-        <v>860</v>
+        <v>854</v>
       </c>
     </row>
     <row r="265">
@@ -6747,10 +6753,10 @@
         <v>732</v>
       </c>
       <c r="H265">
-        <v>17221</v>
+        <v>13146</v>
       </c>
       <c r="I265">
-        <v>854</v>
+        <v>676</v>
       </c>
     </row>
     <row r="266">
@@ -6776,10 +6782,10 @@
         <v>749</v>
       </c>
       <c r="H266">
-        <v>13146</v>
+        <v>13970</v>
       </c>
       <c r="I266">
-        <v>676</v>
+        <v>809</v>
       </c>
     </row>
     <row r="267">
@@ -6805,10 +6811,10 @@
         <v>771</v>
       </c>
       <c r="H267">
-        <v>13970</v>
+        <v>15183</v>
       </c>
       <c r="I267">
-        <v>809</v>
+        <v>716</v>
       </c>
     </row>
     <row r="268">
@@ -6834,10 +6840,10 @@
         <v>798</v>
       </c>
       <c r="H268">
-        <v>15183</v>
+        <v>9461</v>
       </c>
       <c r="I268">
-        <v>716</v>
+        <v>413</v>
       </c>
     </row>
     <row r="269">
@@ -6863,10 +6869,10 @@
         <v>816</v>
       </c>
       <c r="H269">
-        <v>9461</v>
+        <v>2672</v>
       </c>
       <c r="I269">
-        <v>413</v>
+        <v>177</v>
       </c>
     </row>
     <row r="270">
@@ -6892,10 +6898,10 @@
         <v>839</v>
       </c>
       <c r="H270">
-        <v>2672</v>
+        <v>41562</v>
       </c>
       <c r="I270">
-        <v>177</v>
+        <v>1537</v>
       </c>
     </row>
     <row r="271">
@@ -6921,10 +6927,10 @@
         <v>868</v>
       </c>
       <c r="H271">
-        <v>41562</v>
+        <v>30827</v>
       </c>
       <c r="I271">
-        <v>1537</v>
+        <v>1693</v>
       </c>
     </row>
     <row r="272">
@@ -6950,10 +6956,10 @@
         <v>898</v>
       </c>
       <c r="H272">
-        <v>30827</v>
+        <v>25977</v>
       </c>
       <c r="I272">
-        <v>1693</v>
+        <v>1301</v>
       </c>
     </row>
     <row r="273">
@@ -6979,10 +6985,10 @@
         <v>930</v>
       </c>
       <c r="H273">
-        <v>25977</v>
+        <v>27350</v>
       </c>
       <c r="I273">
-        <v>1301</v>
+        <v>1260</v>
       </c>
     </row>
     <row r="274">
@@ -7008,10 +7014,10 @@
         <v>957</v>
       </c>
       <c r="H274">
-        <v>27350</v>
+        <v>27135</v>
       </c>
       <c r="I274">
-        <v>1260</v>
+        <v>1176</v>
       </c>
     </row>
     <row r="275">
@@ -7037,10 +7043,10 @@
         <v>981</v>
       </c>
       <c r="H275">
-        <v>27135</v>
+        <v>12360</v>
       </c>
       <c r="I275">
-        <v>1176</v>
+        <v>400</v>
       </c>
     </row>
     <row r="276">
@@ -7066,10 +7072,10 @@
         <v>996</v>
       </c>
       <c r="H276">
-        <v>12360</v>
+        <v>3069</v>
       </c>
       <c r="I276">
-        <v>400</v>
+        <v>120</v>
       </c>
     </row>
     <row r="277">
@@ -7095,10 +7101,10 @@
         <v>1018</v>
       </c>
       <c r="H277">
-        <v>3069</v>
+        <v>29022</v>
       </c>
       <c r="I277">
-        <v>120</v>
+        <v>1977</v>
       </c>
     </row>
     <row r="278">
@@ -7124,10 +7130,10 @@
         <v>1046</v>
       </c>
       <c r="H278">
-        <v>29022</v>
+        <v>42220</v>
       </c>
       <c r="I278">
-        <v>1977</v>
+        <v>2946</v>
       </c>
     </row>
     <row r="279">
@@ -7153,10 +7159,10 @@
         <v>1084</v>
       </c>
       <c r="H279">
-        <v>42220</v>
+        <v>32670</v>
       </c>
       <c r="I279">
-        <v>2946</v>
+        <v>2130</v>
       </c>
     </row>
     <row r="280">
@@ -7182,10 +7188,10 @@
         <v>1104</v>
       </c>
       <c r="H280">
-        <v>32670</v>
+        <v>41769</v>
       </c>
       <c r="I280">
-        <v>2130</v>
+        <v>2948</v>
       </c>
     </row>
     <row r="281">
@@ -7211,10 +7217,10 @@
         <v>1122</v>
       </c>
       <c r="H281">
-        <v>41769</v>
+        <v>42696</v>
       </c>
       <c r="I281">
-        <v>2948</v>
+        <v>2581</v>
       </c>
     </row>
     <row r="282">
@@ -7240,10 +7246,10 @@
         <v>1148</v>
       </c>
       <c r="H282">
-        <v>42696</v>
+        <v>16398</v>
       </c>
       <c r="I282">
-        <v>2581</v>
+        <v>951</v>
       </c>
     </row>
     <row r="283">
@@ -7269,10 +7275,10 @@
         <v>1175</v>
       </c>
       <c r="H283">
-        <v>16398</v>
+        <v>1509</v>
       </c>
       <c r="I283">
-        <v>951</v>
+        <v>118</v>
       </c>
     </row>
     <row r="284">
@@ -7298,10 +7304,10 @@
         <v>1205</v>
       </c>
       <c r="H284">
-        <v>1509</v>
+        <v>33530</v>
       </c>
       <c r="I284">
-        <v>118</v>
+        <v>2696</v>
       </c>
     </row>
     <row r="285">
@@ -7327,10 +7333,33 @@
         <v>1251</v>
       </c>
       <c r="H285">
-        <v>33530</v>
+        <v>19328</v>
       </c>
       <c r="I285">
-        <v>2696</v>
+        <v>1635</v>
+      </c>
+    </row>
+    <row r="286">
+      <c r="A286" s="2">
+        <v>44180</v>
+      </c>
+      <c r="B286">
+        <v>139088</v>
+      </c>
+      <c r="C286">
+        <v>101584</v>
+      </c>
+      <c r="D286">
+        <v>36195</v>
+      </c>
+      <c r="E286">
+        <v>16717</v>
+      </c>
+      <c r="F286">
+        <v>3565</v>
+      </c>
+      <c r="G286">
+        <v>1309</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated: št 17. 12. 2020
</commit_message>
<xml_diff>
--- a/OpenData_Slovakia_Covid_DailyStats.xlsx
+++ b/OpenData_Slovakia_Covid_DailyStats.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I286"/>
+  <dimension ref="A1:I287"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -6979,7 +6979,7 @@
         <v>930</v>
       </c>
       <c r="H273">
-        <v>25977</v>
+        <v>26052</v>
       </c>
       <c r="I273">
         <v>1301</v>
@@ -7008,10 +7008,10 @@
         <v>957</v>
       </c>
       <c r="H274">
-        <v>27350</v>
+        <v>27352</v>
       </c>
       <c r="I274">
-        <v>1260</v>
+        <v>1262</v>
       </c>
     </row>
     <row r="275">
@@ -7037,10 +7037,10 @@
         <v>981</v>
       </c>
       <c r="H275">
-        <v>27135</v>
+        <v>27416</v>
       </c>
       <c r="I275">
-        <v>1176</v>
+        <v>1186</v>
       </c>
     </row>
     <row r="276">
@@ -7066,10 +7066,10 @@
         <v>996</v>
       </c>
       <c r="H276">
-        <v>12360</v>
+        <v>12551</v>
       </c>
       <c r="I276">
-        <v>400</v>
+        <v>424</v>
       </c>
     </row>
     <row r="277">
@@ -7124,10 +7124,10 @@
         <v>1046</v>
       </c>
       <c r="H278">
-        <v>29022</v>
+        <v>28741</v>
       </c>
       <c r="I278">
-        <v>1977</v>
+        <v>1957</v>
       </c>
     </row>
     <row r="279">
@@ -7153,10 +7153,10 @@
         <v>1084</v>
       </c>
       <c r="H279">
-        <v>42220</v>
+        <v>42606</v>
       </c>
       <c r="I279">
-        <v>2946</v>
+        <v>3008</v>
       </c>
     </row>
     <row r="280">
@@ -7182,10 +7182,10 @@
         <v>1104</v>
       </c>
       <c r="H280">
-        <v>32670</v>
+        <v>33854</v>
       </c>
       <c r="I280">
-        <v>2130</v>
+        <v>2244</v>
       </c>
     </row>
     <row r="281">
@@ -7211,10 +7211,10 @@
         <v>1122</v>
       </c>
       <c r="H281">
-        <v>41769</v>
+        <v>42544</v>
       </c>
       <c r="I281">
-        <v>2948</v>
+        <v>3040</v>
       </c>
     </row>
     <row r="282">
@@ -7240,10 +7240,10 @@
         <v>1148</v>
       </c>
       <c r="H282">
-        <v>42696</v>
+        <v>43293</v>
       </c>
       <c r="I282">
-        <v>2581</v>
+        <v>2612</v>
       </c>
     </row>
     <row r="283">
@@ -7269,10 +7269,10 @@
         <v>1175</v>
       </c>
       <c r="H283">
-        <v>16398</v>
+        <v>16537</v>
       </c>
       <c r="I283">
-        <v>951</v>
+        <v>960</v>
       </c>
     </row>
     <row r="284">
@@ -7298,10 +7298,10 @@
         <v>1205</v>
       </c>
       <c r="H284">
-        <v>1509</v>
+        <v>1357</v>
       </c>
       <c r="I284">
-        <v>118</v>
+        <v>114</v>
       </c>
     </row>
     <row r="285">
@@ -7327,10 +7327,10 @@
         <v>1251</v>
       </c>
       <c r="H285">
-        <v>33530</v>
+        <v>37513</v>
       </c>
       <c r="I285">
-        <v>2696</v>
+        <v>3065</v>
       </c>
     </row>
     <row r="286">
@@ -7356,10 +7356,39 @@
         <v>1309</v>
       </c>
       <c r="H286">
-        <v>19328</v>
+        <v>50718</v>
       </c>
       <c r="I286">
-        <v>1635</v>
+        <v>3793</v>
+      </c>
+    </row>
+    <row r="287">
+      <c r="A287" s="2">
+        <v>44181</v>
+      </c>
+      <c r="B287">
+        <v>142133</v>
+      </c>
+      <c r="C287">
+        <v>102737</v>
+      </c>
+      <c r="D287">
+        <v>38018</v>
+      </c>
+      <c r="E287">
+        <v>14921</v>
+      </c>
+      <c r="F287">
+        <v>3045</v>
+      </c>
+      <c r="G287">
+        <v>1378</v>
+      </c>
+      <c r="H287">
+        <v>49741</v>
+      </c>
+      <c r="I287">
+        <v>3369</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated: ut 22. 12. 2020
</commit_message>
<xml_diff>
--- a/OpenData_Slovakia_Covid_DailyStats.xlsx
+++ b/OpenData_Slovakia_Covid_DailyStats.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I287"/>
+  <dimension ref="A1:I291"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -6515,10 +6515,10 @@
         <v>557</v>
       </c>
       <c r="H257">
-        <v>5258</v>
+        <v>5229</v>
       </c>
       <c r="I257">
-        <v>275</v>
+        <v>273</v>
       </c>
     </row>
     <row r="258">
@@ -6544,10 +6544,10 @@
         <v>579</v>
       </c>
       <c r="H258">
-        <v>3874</v>
+        <v>3860</v>
       </c>
       <c r="I258">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="259">
@@ -6573,10 +6573,10 @@
         <v>579</v>
       </c>
       <c r="H259">
-        <v>6114</v>
+        <v>6103</v>
       </c>
       <c r="I259">
-        <v>423</v>
+        <v>419</v>
       </c>
     </row>
     <row r="260">
@@ -6602,10 +6602,10 @@
         <v>614</v>
       </c>
       <c r="H260">
-        <v>11540</v>
+        <v>11479</v>
       </c>
       <c r="I260">
-        <v>750</v>
+        <v>746</v>
       </c>
     </row>
     <row r="261">
@@ -6631,10 +6631,10 @@
         <v>644</v>
       </c>
       <c r="H261">
-        <v>17458</v>
+        <v>17378</v>
       </c>
       <c r="I261">
-        <v>597</v>
+        <v>596</v>
       </c>
     </row>
     <row r="262">
@@ -6660,7 +6660,7 @@
         <v>671</v>
       </c>
       <c r="H262">
-        <v>9226</v>
+        <v>9215</v>
       </c>
       <c r="I262">
         <v>317</v>
@@ -6718,10 +6718,10 @@
         <v>709</v>
       </c>
       <c r="H264">
-        <v>42064</v>
+        <v>41901</v>
       </c>
       <c r="I264">
-        <v>860</v>
+        <v>845</v>
       </c>
     </row>
     <row r="265">
@@ -6747,7 +6747,7 @@
         <v>732</v>
       </c>
       <c r="H265">
-        <v>17221</v>
+        <v>17198</v>
       </c>
       <c r="I265">
         <v>854</v>
@@ -6776,10 +6776,10 @@
         <v>749</v>
       </c>
       <c r="H266">
-        <v>13146</v>
+        <v>13085</v>
       </c>
       <c r="I266">
-        <v>676</v>
+        <v>671</v>
       </c>
     </row>
     <row r="267">
@@ -6805,10 +6805,10 @@
         <v>771</v>
       </c>
       <c r="H267">
-        <v>13970</v>
+        <v>13894</v>
       </c>
       <c r="I267">
-        <v>809</v>
+        <v>807</v>
       </c>
     </row>
     <row r="268">
@@ -6834,10 +6834,10 @@
         <v>798</v>
       </c>
       <c r="H268">
-        <v>15183</v>
+        <v>15137</v>
       </c>
       <c r="I268">
-        <v>716</v>
+        <v>714</v>
       </c>
     </row>
     <row r="269">
@@ -6863,10 +6863,10 @@
         <v>816</v>
       </c>
       <c r="H269">
-        <v>9461</v>
+        <v>9451</v>
       </c>
       <c r="I269">
-        <v>413</v>
+        <v>411</v>
       </c>
     </row>
     <row r="270">
@@ -6921,10 +6921,10 @@
         <v>868</v>
       </c>
       <c r="H271">
-        <v>41562</v>
+        <v>42085</v>
       </c>
       <c r="I271">
-        <v>1537</v>
+        <v>1592</v>
       </c>
     </row>
     <row r="272">
@@ -6950,10 +6950,10 @@
         <v>898</v>
       </c>
       <c r="H272">
-        <v>30827</v>
+        <v>30464</v>
       </c>
       <c r="I272">
-        <v>1693</v>
+        <v>1641</v>
       </c>
     </row>
     <row r="273">
@@ -6979,10 +6979,10 @@
         <v>930</v>
       </c>
       <c r="H273">
-        <v>26052</v>
+        <v>26705</v>
       </c>
       <c r="I273">
-        <v>1301</v>
+        <v>1358</v>
       </c>
     </row>
     <row r="274">
@@ -7008,10 +7008,10 @@
         <v>957</v>
       </c>
       <c r="H274">
-        <v>27352</v>
+        <v>28086</v>
       </c>
       <c r="I274">
-        <v>1262</v>
+        <v>1309</v>
       </c>
     </row>
     <row r="275">
@@ -7037,10 +7037,10 @@
         <v>981</v>
       </c>
       <c r="H275">
-        <v>27416</v>
+        <v>28515</v>
       </c>
       <c r="I275">
-        <v>1186</v>
+        <v>1243</v>
       </c>
     </row>
     <row r="276">
@@ -7066,10 +7066,10 @@
         <v>996</v>
       </c>
       <c r="H276">
-        <v>12551</v>
+        <v>13858</v>
       </c>
       <c r="I276">
-        <v>424</v>
+        <v>459</v>
       </c>
     </row>
     <row r="277">
@@ -7095,10 +7095,10 @@
         <v>1018</v>
       </c>
       <c r="H277">
-        <v>3069</v>
+        <v>3252</v>
       </c>
       <c r="I277">
-        <v>120</v>
+        <v>125</v>
       </c>
     </row>
     <row r="278">
@@ -7124,10 +7124,10 @@
         <v>1046</v>
       </c>
       <c r="H278">
-        <v>28741</v>
+        <v>29445</v>
       </c>
       <c r="I278">
-        <v>1957</v>
+        <v>2022</v>
       </c>
     </row>
     <row r="279">
@@ -7153,10 +7153,10 @@
         <v>1084</v>
       </c>
       <c r="H279">
-        <v>42606</v>
+        <v>44046</v>
       </c>
       <c r="I279">
-        <v>3008</v>
+        <v>3121</v>
       </c>
     </row>
     <row r="280">
@@ -7182,10 +7182,10 @@
         <v>1104</v>
       </c>
       <c r="H280">
-        <v>33854</v>
+        <v>35947</v>
       </c>
       <c r="I280">
-        <v>2244</v>
+        <v>2382</v>
       </c>
     </row>
     <row r="281">
@@ -7211,10 +7211,10 @@
         <v>1122</v>
       </c>
       <c r="H281">
-        <v>42544</v>
+        <v>44974</v>
       </c>
       <c r="I281">
-        <v>3040</v>
+        <v>3255</v>
       </c>
     </row>
     <row r="282">
@@ -7240,10 +7240,10 @@
         <v>1148</v>
       </c>
       <c r="H282">
-        <v>43293</v>
+        <v>46434</v>
       </c>
       <c r="I282">
-        <v>2612</v>
+        <v>2821</v>
       </c>
     </row>
     <row r="283">
@@ -7269,10 +7269,10 @@
         <v>1175</v>
       </c>
       <c r="H283">
-        <v>16537</v>
+        <v>17661</v>
       </c>
       <c r="I283">
-        <v>960</v>
+        <v>1043</v>
       </c>
     </row>
     <row r="284">
@@ -7298,10 +7298,10 @@
         <v>1205</v>
       </c>
       <c r="H284">
-        <v>1357</v>
+        <v>1090</v>
       </c>
       <c r="I284">
-        <v>114</v>
+        <v>95</v>
       </c>
     </row>
     <row r="285">
@@ -7327,10 +7327,10 @@
         <v>1251</v>
       </c>
       <c r="H285">
-        <v>37513</v>
+        <v>40066</v>
       </c>
       <c r="I285">
-        <v>3065</v>
+        <v>3374</v>
       </c>
     </row>
     <row r="286">
@@ -7356,10 +7356,10 @@
         <v>1309</v>
       </c>
       <c r="H286">
-        <v>50718</v>
+        <v>54412</v>
       </c>
       <c r="I286">
-        <v>3793</v>
+        <v>4146</v>
       </c>
     </row>
     <row r="287">
@@ -7385,10 +7385,126 @@
         <v>1378</v>
       </c>
       <c r="H287">
-        <v>49741</v>
+        <v>55695</v>
       </c>
       <c r="I287">
-        <v>3369</v>
+        <v>3766</v>
+      </c>
+    </row>
+    <row r="288">
+      <c r="A288" s="2">
+        <v>44182</v>
+      </c>
+      <c r="B288">
+        <v>146124</v>
+      </c>
+      <c r="C288">
+        <v>104560</v>
+      </c>
+      <c r="D288">
+        <v>40124</v>
+      </c>
+      <c r="E288">
+        <v>18022</v>
+      </c>
+      <c r="F288">
+        <v>3991</v>
+      </c>
+      <c r="G288">
+        <v>1440</v>
+      </c>
+      <c r="H288">
+        <v>52854</v>
+      </c>
+      <c r="I288">
+        <v>3878</v>
+      </c>
+    </row>
+    <row r="289">
+      <c r="A289" s="2">
+        <v>44183</v>
+      </c>
+      <c r="B289">
+        <v>149275</v>
+      </c>
+      <c r="C289">
+        <v>106361</v>
+      </c>
+      <c r="D289">
+        <v>41404</v>
+      </c>
+      <c r="E289">
+        <v>16197</v>
+      </c>
+      <c r="F289">
+        <v>3151</v>
+      </c>
+      <c r="G289">
+        <v>1510</v>
+      </c>
+      <c r="H289">
+        <v>61403</v>
+      </c>
+      <c r="I289">
+        <v>3500</v>
+      </c>
+    </row>
+    <row r="290">
+      <c r="A290" s="2">
+        <v>44184</v>
+      </c>
+      <c r="B290">
+        <v>151336</v>
+      </c>
+      <c r="C290">
+        <v>107828</v>
+      </c>
+      <c r="D290">
+        <v>41953</v>
+      </c>
+      <c r="E290">
+        <v>9821</v>
+      </c>
+      <c r="F290">
+        <v>2061</v>
+      </c>
+      <c r="G290">
+        <v>1555</v>
+      </c>
+      <c r="H290">
+        <v>18289</v>
+      </c>
+      <c r="I290">
+        <v>1500</v>
+      </c>
+    </row>
+    <row r="291">
+      <c r="A291" s="2">
+        <v>44185</v>
+      </c>
+      <c r="B291">
+        <v>152555</v>
+      </c>
+      <c r="C291">
+        <v>109807</v>
+      </c>
+      <c r="D291">
+        <v>41130</v>
+      </c>
+      <c r="E291">
+        <v>6291</v>
+      </c>
+      <c r="F291">
+        <v>1219</v>
+      </c>
+      <c r="G291">
+        <v>1618</v>
+      </c>
+      <c r="H291">
+        <v>14351</v>
+      </c>
+      <c r="I291">
+        <v>458</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated: po 28. 12. 2020
</commit_message>
<xml_diff>
--- a/OpenData_Slovakia_Covid_DailyStats.xlsx
+++ b/OpenData_Slovakia_Covid_DailyStats.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I293"/>
+  <dimension ref="A1:I298"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -6950,7 +6950,7 @@
         <v>898</v>
       </c>
       <c r="H272">
-        <v>30632</v>
+        <v>30644</v>
       </c>
       <c r="I272">
         <v>1650</v>
@@ -7066,7 +7066,7 @@
         <v>996</v>
       </c>
       <c r="H276">
-        <v>13291</v>
+        <v>13295</v>
       </c>
       <c r="I276">
         <v>454</v>
@@ -7095,7 +7095,7 @@
         <v>1018</v>
       </c>
       <c r="H277">
-        <v>3209</v>
+        <v>3222</v>
       </c>
       <c r="I277">
         <v>125</v>
@@ -7124,7 +7124,7 @@
         <v>1046</v>
       </c>
       <c r="H278">
-        <v>29958</v>
+        <v>29967</v>
       </c>
       <c r="I278">
         <v>2086</v>
@@ -7153,10 +7153,10 @@
         <v>1084</v>
       </c>
       <c r="H279">
-        <v>43610</v>
+        <v>42294</v>
       </c>
       <c r="I279">
-        <v>3099</v>
+        <v>3080</v>
       </c>
     </row>
     <row r="280">
@@ -7182,7 +7182,7 @@
         <v>1104</v>
       </c>
       <c r="H280">
-        <v>35941</v>
+        <v>35942</v>
       </c>
       <c r="I280">
         <v>2392</v>
@@ -7211,7 +7211,7 @@
         <v>1122</v>
       </c>
       <c r="H281">
-        <v>45611</v>
+        <v>45614</v>
       </c>
       <c r="I281">
         <v>3298</v>
@@ -7240,10 +7240,10 @@
         <v>1148</v>
       </c>
       <c r="H282">
-        <v>46588</v>
+        <v>46593</v>
       </c>
       <c r="I282">
-        <v>2836</v>
+        <v>2837</v>
       </c>
     </row>
     <row r="283">
@@ -7298,7 +7298,7 @@
         <v>1205</v>
       </c>
       <c r="H284">
-        <v>1090</v>
+        <v>1095</v>
       </c>
       <c r="I284">
         <v>95</v>
@@ -7327,7 +7327,7 @@
         <v>1251</v>
       </c>
       <c r="H285">
-        <v>40414</v>
+        <v>40447</v>
       </c>
       <c r="I285">
         <v>3411</v>
@@ -7356,10 +7356,10 @@
         <v>1309</v>
       </c>
       <c r="H286">
-        <v>54605</v>
+        <v>54756</v>
       </c>
       <c r="I286">
-        <v>4184</v>
+        <v>4187</v>
       </c>
     </row>
     <row r="287">
@@ -7385,10 +7385,10 @@
         <v>1378</v>
       </c>
       <c r="H287">
-        <v>56879</v>
+        <v>57298</v>
       </c>
       <c r="I287">
-        <v>3880</v>
+        <v>3902</v>
       </c>
     </row>
     <row r="288">
@@ -7414,10 +7414,10 @@
         <v>1440</v>
       </c>
       <c r="H288">
-        <v>53854</v>
+        <v>56222</v>
       </c>
       <c r="I288">
-        <v>3923</v>
+        <v>4102</v>
       </c>
     </row>
     <row r="289">
@@ -7443,10 +7443,10 @@
         <v>1510</v>
       </c>
       <c r="H289">
-        <v>62747</v>
+        <v>64269</v>
       </c>
       <c r="I289">
-        <v>3619</v>
+        <v>4348</v>
       </c>
     </row>
     <row r="290">
@@ -7472,10 +7472,10 @@
         <v>1555</v>
       </c>
       <c r="H290">
-        <v>18289</v>
+        <v>18292</v>
       </c>
       <c r="I290">
-        <v>1500</v>
+        <v>1501</v>
       </c>
     </row>
     <row r="291">
@@ -7530,10 +7530,10 @@
         <v>1618</v>
       </c>
       <c r="H292">
-        <v>76465</v>
+        <v>78191</v>
       </c>
       <c r="I292">
-        <v>6710</v>
+        <v>6924</v>
       </c>
     </row>
     <row r="293">
@@ -7559,10 +7559,155 @@
         <v>1686</v>
       </c>
       <c r="H293">
-        <v>73961</v>
+        <v>78922</v>
       </c>
       <c r="I293">
-        <v>5349</v>
+        <v>5663</v>
+      </c>
+    </row>
+    <row r="294">
+      <c r="A294" s="2">
+        <v>44188</v>
+      </c>
+      <c r="B294">
+        <v>161562</v>
+      </c>
+      <c r="C294">
+        <v>114267</v>
+      </c>
+      <c r="D294">
+        <v>45563</v>
+      </c>
+      <c r="E294">
+        <v>14238</v>
+      </c>
+      <c r="F294">
+        <v>2657</v>
+      </c>
+      <c r="G294">
+        <v>1732</v>
+      </c>
+      <c r="H294">
+        <v>86638</v>
+      </c>
+      <c r="I294">
+        <v>4784</v>
+      </c>
+    </row>
+    <row r="295">
+      <c r="A295" s="2">
+        <v>44189</v>
+      </c>
+      <c r="B295">
+        <v>165608</v>
+      </c>
+      <c r="C295">
+        <v>115663</v>
+      </c>
+      <c r="D295">
+        <v>48213</v>
+      </c>
+      <c r="E295">
+        <v>18443</v>
+      </c>
+      <c r="F295">
+        <v>4046</v>
+      </c>
+      <c r="G295">
+        <v>1732</v>
+      </c>
+      <c r="H295">
+        <v>19236</v>
+      </c>
+      <c r="I295">
+        <v>1136</v>
+      </c>
+    </row>
+    <row r="296">
+      <c r="A296" s="2">
+        <v>44190</v>
+      </c>
+      <c r="B296">
+        <v>166649</v>
+      </c>
+      <c r="C296">
+        <v>116948</v>
+      </c>
+      <c r="D296">
+        <v>47969</v>
+      </c>
+      <c r="E296">
+        <v>4249</v>
+      </c>
+      <c r="F296">
+        <v>1041</v>
+      </c>
+      <c r="G296">
+        <v>1732</v>
+      </c>
+      <c r="H296">
+        <v>1853</v>
+      </c>
+      <c r="I296">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="297">
+      <c r="A297" s="2">
+        <v>44191</v>
+      </c>
+      <c r="B297">
+        <v>167523</v>
+      </c>
+      <c r="C297">
+        <v>119086</v>
+      </c>
+      <c r="D297">
+        <v>46664</v>
+      </c>
+      <c r="E297">
+        <v>3550</v>
+      </c>
+      <c r="F297">
+        <v>874</v>
+      </c>
+      <c r="G297">
+        <v>1773</v>
+      </c>
+      <c r="H297">
+        <v>2568</v>
+      </c>
+      <c r="I297">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="298">
+      <c r="A298" s="2">
+        <v>44192</v>
+      </c>
+      <c r="B298">
+        <v>168092</v>
+      </c>
+      <c r="C298">
+        <v>120410</v>
+      </c>
+      <c r="D298">
+        <v>45803</v>
+      </c>
+      <c r="E298">
+        <v>2540</v>
+      </c>
+      <c r="F298">
+        <v>569</v>
+      </c>
+      <c r="G298">
+        <v>1879</v>
+      </c>
+      <c r="H298">
+        <v>2462</v>
+      </c>
+      <c r="I298">
+        <v>250</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated: ut 29. 12. 2020
</commit_message>
<xml_diff>
--- a/OpenData_Slovakia_Covid_DailyStats.xlsx
+++ b/OpenData_Slovakia_Covid_DailyStats.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I298"/>
+  <dimension ref="A1:I299"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -7710,6 +7710,35 @@
         <v>250</v>
       </c>
     </row>
+    <row r="299">
+      <c r="A299" s="2">
+        <v>44193</v>
+      </c>
+      <c r="B299">
+        <v>170187</v>
+      </c>
+      <c r="C299">
+        <v>121760</v>
+      </c>
+      <c r="D299">
+        <v>46444</v>
+      </c>
+      <c r="E299">
+        <v>9330</v>
+      </c>
+      <c r="F299">
+        <v>2095</v>
+      </c>
+      <c r="G299">
+        <v>1983</v>
+      </c>
+      <c r="H299">
+        <v>13032</v>
+      </c>
+      <c r="I299">
+        <v>998</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated: št 31. 12. 2020
</commit_message>
<xml_diff>
--- a/OpenData_Slovakia_Covid_DailyStats.xlsx
+++ b/OpenData_Slovakia_Covid_DailyStats.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I299"/>
+  <dimension ref="A1:I301"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -6776,10 +6776,10 @@
         <v>749</v>
       </c>
       <c r="H266">
-        <v>13085</v>
+        <v>12665</v>
       </c>
       <c r="I266">
-        <v>671</v>
+        <v>664</v>
       </c>
     </row>
     <row r="267">
@@ -6805,10 +6805,10 @@
         <v>771</v>
       </c>
       <c r="H267">
-        <v>13894</v>
+        <v>13318</v>
       </c>
       <c r="I267">
-        <v>807</v>
+        <v>791</v>
       </c>
     </row>
     <row r="268">
@@ -6834,10 +6834,10 @@
         <v>798</v>
       </c>
       <c r="H268">
-        <v>15137</v>
+        <v>14407</v>
       </c>
       <c r="I268">
-        <v>714</v>
+        <v>697</v>
       </c>
     </row>
     <row r="269">
@@ -6863,10 +6863,10 @@
         <v>816</v>
       </c>
       <c r="H269">
-        <v>9451</v>
+        <v>8811</v>
       </c>
       <c r="I269">
-        <v>411</v>
+        <v>399</v>
       </c>
     </row>
     <row r="270">
@@ -6892,10 +6892,10 @@
         <v>839</v>
       </c>
       <c r="H270">
-        <v>2672</v>
+        <v>2517</v>
       </c>
       <c r="I270">
-        <v>177</v>
+        <v>174</v>
       </c>
     </row>
     <row r="271">
@@ -6921,10 +6921,10 @@
         <v>868</v>
       </c>
       <c r="H271">
-        <v>42446</v>
+        <v>42454</v>
       </c>
       <c r="I271">
-        <v>1612</v>
+        <v>1616</v>
       </c>
     </row>
     <row r="272">
@@ -6950,7 +6950,7 @@
         <v>898</v>
       </c>
       <c r="H272">
-        <v>30655</v>
+        <v>30658</v>
       </c>
       <c r="I272">
         <v>1650</v>
@@ -6979,7 +6979,7 @@
         <v>930</v>
       </c>
       <c r="H273">
-        <v>26904</v>
+        <v>26905</v>
       </c>
       <c r="I273">
         <v>1366</v>
@@ -7008,7 +7008,7 @@
         <v>957</v>
       </c>
       <c r="H274">
-        <v>28359</v>
+        <v>28368</v>
       </c>
       <c r="I274">
         <v>1338</v>
@@ -7211,7 +7211,7 @@
         <v>1122</v>
       </c>
       <c r="H281">
-        <v>45260</v>
+        <v>45270</v>
       </c>
       <c r="I281">
         <v>3262</v>
@@ -7240,10 +7240,10 @@
         <v>1148</v>
       </c>
       <c r="H282">
-        <v>46722</v>
+        <v>46880</v>
       </c>
       <c r="I282">
-        <v>2841</v>
+        <v>2853</v>
       </c>
     </row>
     <row r="283">
@@ -7327,10 +7327,10 @@
         <v>1251</v>
       </c>
       <c r="H285">
-        <v>40447</v>
+        <v>40827</v>
       </c>
       <c r="I285">
-        <v>3411</v>
+        <v>3423</v>
       </c>
     </row>
     <row r="286">
@@ -7356,10 +7356,10 @@
         <v>1309</v>
       </c>
       <c r="H286">
-        <v>54599</v>
+        <v>55096</v>
       </c>
       <c r="I286">
-        <v>4223</v>
+        <v>4238</v>
       </c>
     </row>
     <row r="287">
@@ -7385,10 +7385,10 @@
         <v>1378</v>
       </c>
       <c r="H287">
-        <v>56340</v>
+        <v>57236</v>
       </c>
       <c r="I287">
-        <v>3842</v>
+        <v>3902</v>
       </c>
     </row>
     <row r="288">
@@ -7414,10 +7414,10 @@
         <v>1440</v>
       </c>
       <c r="H288">
-        <v>55543</v>
+        <v>56606</v>
       </c>
       <c r="I288">
-        <v>3939</v>
+        <v>3985</v>
       </c>
     </row>
     <row r="289">
@@ -7443,10 +7443,10 @@
         <v>1510</v>
       </c>
       <c r="H289">
-        <v>63085</v>
+        <v>64580</v>
       </c>
       <c r="I289">
-        <v>3575</v>
+        <v>3648</v>
       </c>
     </row>
     <row r="290">
@@ -7530,10 +7530,10 @@
         <v>1618</v>
       </c>
       <c r="H292">
-        <v>77798</v>
+        <v>80096</v>
       </c>
       <c r="I292">
-        <v>6926</v>
+        <v>7078</v>
       </c>
     </row>
     <row r="293">
@@ -7559,10 +7559,10 @@
         <v>1686</v>
       </c>
       <c r="H293">
-        <v>78690</v>
+        <v>81616</v>
       </c>
       <c r="I293">
-        <v>5669</v>
+        <v>5776</v>
       </c>
     </row>
     <row r="294">
@@ -7588,10 +7588,10 @@
         <v>1732</v>
       </c>
       <c r="H294">
-        <v>87303</v>
+        <v>90143</v>
       </c>
       <c r="I294">
-        <v>4828</v>
+        <v>4928</v>
       </c>
     </row>
     <row r="295">
@@ -7617,7 +7617,7 @@
         <v>1732</v>
       </c>
       <c r="H295">
-        <v>19248</v>
+        <v>19252</v>
       </c>
       <c r="I295">
         <v>1136</v>
@@ -7675,10 +7675,10 @@
         <v>1773</v>
       </c>
       <c r="H297">
-        <v>2572</v>
+        <v>2648</v>
       </c>
       <c r="I297">
-        <v>228</v>
+        <v>232</v>
       </c>
     </row>
     <row r="298">
@@ -7704,10 +7704,10 @@
         <v>1879</v>
       </c>
       <c r="H298">
-        <v>2564</v>
+        <v>3092</v>
       </c>
       <c r="I298">
-        <v>268</v>
+        <v>286</v>
       </c>
     </row>
     <row r="299">
@@ -7733,10 +7733,68 @@
         <v>1983</v>
       </c>
       <c r="H299">
-        <v>57834</v>
+        <v>61986</v>
       </c>
       <c r="I299">
-        <v>6074</v>
+        <v>6418</v>
+      </c>
+    </row>
+    <row r="300">
+      <c r="A300" s="2">
+        <v>44194</v>
+      </c>
+      <c r="B300">
+        <v>173228</v>
+      </c>
+      <c r="C300">
+        <v>124427</v>
+      </c>
+      <c r="D300">
+        <v>46736</v>
+      </c>
+      <c r="E300">
+        <v>11414</v>
+      </c>
+      <c r="F300">
+        <v>3041</v>
+      </c>
+      <c r="G300">
+        <v>2065</v>
+      </c>
+      <c r="H300">
+        <v>66489</v>
+      </c>
+      <c r="I300">
+        <v>6416</v>
+      </c>
+    </row>
+    <row r="301">
+      <c r="A301" s="2">
+        <v>44195</v>
+      </c>
+      <c r="B301">
+        <v>179543</v>
+      </c>
+      <c r="C301">
+        <v>125971</v>
+      </c>
+      <c r="D301">
+        <v>51434</v>
+      </c>
+      <c r="E301">
+        <v>21978</v>
+      </c>
+      <c r="F301">
+        <v>6315</v>
+      </c>
+      <c r="G301">
+        <v>2138</v>
+      </c>
+      <c r="H301">
+        <v>63851</v>
+      </c>
+      <c r="I301">
+        <v>5118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated: po 04. 01. 2021
</commit_message>
<xml_diff>
--- a/OpenData_Slovakia_Covid_DailyStats.xlsx
+++ b/OpenData_Slovakia_Covid_DailyStats.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I301"/>
+  <dimension ref="A1:I305"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -7240,7 +7240,7 @@
         <v>1148</v>
       </c>
       <c r="H282">
-        <v>46880</v>
+        <v>46903</v>
       </c>
       <c r="I282">
         <v>2853</v>
@@ -7327,10 +7327,10 @@
         <v>1251</v>
       </c>
       <c r="H285">
-        <v>40827</v>
+        <v>40950</v>
       </c>
       <c r="I285">
-        <v>3423</v>
+        <v>3441</v>
       </c>
     </row>
     <row r="286">
@@ -7356,10 +7356,10 @@
         <v>1309</v>
       </c>
       <c r="H286">
-        <v>55096</v>
+        <v>55412</v>
       </c>
       <c r="I286">
-        <v>4238</v>
+        <v>4260</v>
       </c>
     </row>
     <row r="287">
@@ -7385,10 +7385,10 @@
         <v>1378</v>
       </c>
       <c r="H287">
-        <v>57236</v>
+        <v>57336</v>
       </c>
       <c r="I287">
-        <v>3902</v>
+        <v>3911</v>
       </c>
     </row>
     <row r="288">
@@ -7414,10 +7414,10 @@
         <v>1440</v>
       </c>
       <c r="H288">
-        <v>56606</v>
+        <v>57178</v>
       </c>
       <c r="I288">
-        <v>3985</v>
+        <v>4008</v>
       </c>
     </row>
     <row r="289">
@@ -7443,10 +7443,10 @@
         <v>1510</v>
       </c>
       <c r="H289">
-        <v>64580</v>
+        <v>64737</v>
       </c>
       <c r="I289">
-        <v>3648</v>
+        <v>3666</v>
       </c>
     </row>
     <row r="290">
@@ -7530,10 +7530,10 @@
         <v>1618</v>
       </c>
       <c r="H292">
-        <v>80096</v>
+        <v>80874</v>
       </c>
       <c r="I292">
-        <v>7078</v>
+        <v>7159</v>
       </c>
     </row>
     <row r="293">
@@ -7559,10 +7559,10 @@
         <v>1686</v>
       </c>
       <c r="H293">
-        <v>81616</v>
+        <v>82398</v>
       </c>
       <c r="I293">
-        <v>5776</v>
+        <v>5860</v>
       </c>
     </row>
     <row r="294">
@@ -7588,10 +7588,10 @@
         <v>1732</v>
       </c>
       <c r="H294">
-        <v>90143</v>
+        <v>90608</v>
       </c>
       <c r="I294">
-        <v>4928</v>
+        <v>4941</v>
       </c>
     </row>
     <row r="295">
@@ -7733,10 +7733,10 @@
         <v>1983</v>
       </c>
       <c r="H299">
-        <v>61986</v>
+        <v>62461</v>
       </c>
       <c r="I299">
-        <v>6418</v>
+        <v>6487</v>
       </c>
     </row>
     <row r="300">
@@ -7762,10 +7762,10 @@
         <v>2065</v>
       </c>
       <c r="H300">
-        <v>66489</v>
+        <v>68069</v>
       </c>
       <c r="I300">
-        <v>6416</v>
+        <v>6628</v>
       </c>
     </row>
     <row r="301">
@@ -7791,10 +7791,126 @@
         <v>2138</v>
       </c>
       <c r="H301">
-        <v>63851</v>
+        <v>64702</v>
       </c>
       <c r="I301">
-        <v>5118</v>
+        <v>5164</v>
+      </c>
+    </row>
+    <row r="302">
+      <c r="A302" s="2">
+        <v>44196</v>
+      </c>
+      <c r="B302">
+        <v>184508</v>
+      </c>
+      <c r="C302">
+        <v>127190</v>
+      </c>
+      <c r="D302">
+        <v>55068</v>
+      </c>
+      <c r="E302">
+        <v>16479</v>
+      </c>
+      <c r="F302">
+        <v>4965</v>
+      </c>
+      <c r="G302">
+        <v>2250</v>
+      </c>
+      <c r="H302">
+        <v>63225</v>
+      </c>
+      <c r="I302">
+        <v>4620</v>
+      </c>
+    </row>
+    <row r="303">
+      <c r="A303" s="2">
+        <v>44197</v>
+      </c>
+      <c r="B303">
+        <v>186244</v>
+      </c>
+      <c r="C303">
+        <v>128285</v>
+      </c>
+      <c r="D303">
+        <v>55709</v>
+      </c>
+      <c r="E303">
+        <v>4954</v>
+      </c>
+      <c r="F303">
+        <v>1736</v>
+      </c>
+      <c r="G303">
+        <v>2250</v>
+      </c>
+      <c r="H303">
+        <v>9566</v>
+      </c>
+      <c r="I303">
+        <v>678</v>
+      </c>
+    </row>
+    <row r="304">
+      <c r="A304" s="2">
+        <v>44198</v>
+      </c>
+      <c r="B304">
+        <v>187463</v>
+      </c>
+      <c r="C304">
+        <v>129994</v>
+      </c>
+      <c r="D304">
+        <v>55152</v>
+      </c>
+      <c r="E304">
+        <v>4288</v>
+      </c>
+      <c r="F304">
+        <v>1219</v>
+      </c>
+      <c r="G304">
+        <v>2317</v>
+      </c>
+      <c r="H304">
+        <v>6388</v>
+      </c>
+      <c r="I304">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="305">
+      <c r="A305" s="2">
+        <v>44199</v>
+      </c>
+      <c r="B305">
+        <v>188099</v>
+      </c>
+      <c r="C305">
+        <v>130897</v>
+      </c>
+      <c r="D305">
+        <v>54681</v>
+      </c>
+      <c r="E305">
+        <v>3111</v>
+      </c>
+      <c r="F305">
+        <v>636</v>
+      </c>
+      <c r="G305">
+        <v>2521</v>
+      </c>
+      <c r="H305">
+        <v>3404</v>
+      </c>
+      <c r="I305">
+        <v>312</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated: ut 05. 01. 2021
</commit_message>
<xml_diff>
--- a/OpenData_Slovakia_Covid_DailyStats.xlsx
+++ b/OpenData_Slovakia_Covid_DailyStats.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I305"/>
+  <dimension ref="A1:I306"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -7913,6 +7913,35 @@
         <v>312</v>
       </c>
     </row>
+    <row r="306">
+      <c r="A306" s="2">
+        <v>44200</v>
+      </c>
+      <c r="B306">
+        <v>191088</v>
+      </c>
+      <c r="C306">
+        <v>132852</v>
+      </c>
+      <c r="D306">
+        <v>55633</v>
+      </c>
+      <c r="E306">
+        <v>12396</v>
+      </c>
+      <c r="F306">
+        <v>2989</v>
+      </c>
+      <c r="G306">
+        <v>2603</v>
+      </c>
+      <c r="H306">
+        <v>8676</v>
+      </c>
+      <c r="I306">
+        <v>600</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updated: št 07. 01. 2021
</commit_message>
<xml_diff>
--- a/OpenData_Slovakia_Covid_DailyStats.xlsx
+++ b/OpenData_Slovakia_Covid_DailyStats.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I306"/>
+  <dimension ref="A1:I308"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -6921,10 +6921,10 @@
         <v>868</v>
       </c>
       <c r="H271">
-        <v>42454</v>
+        <v>42580</v>
       </c>
       <c r="I271">
-        <v>1616</v>
+        <v>1620</v>
       </c>
     </row>
     <row r="272">
@@ -6950,10 +6950,10 @@
         <v>898</v>
       </c>
       <c r="H272">
-        <v>30658</v>
+        <v>30999</v>
       </c>
       <c r="I272">
-        <v>1650</v>
+        <v>1666</v>
       </c>
     </row>
     <row r="273">
@@ -6979,10 +6979,10 @@
         <v>930</v>
       </c>
       <c r="H273">
-        <v>26905</v>
+        <v>27150</v>
       </c>
       <c r="I273">
-        <v>1366</v>
+        <v>1367</v>
       </c>
     </row>
     <row r="274">
@@ -7008,10 +7008,10 @@
         <v>957</v>
       </c>
       <c r="H274">
-        <v>28368</v>
+        <v>28390</v>
       </c>
       <c r="I274">
-        <v>1338</v>
+        <v>1348</v>
       </c>
     </row>
     <row r="275">
@@ -7037,10 +7037,10 @@
         <v>981</v>
       </c>
       <c r="H275">
-        <v>28773</v>
+        <v>28740</v>
       </c>
       <c r="I275">
-        <v>1238</v>
+        <v>1239</v>
       </c>
     </row>
     <row r="276">
@@ -7124,10 +7124,10 @@
         <v>1046</v>
       </c>
       <c r="H278">
-        <v>29664</v>
+        <v>29996</v>
       </c>
       <c r="I278">
-        <v>2056</v>
+        <v>2101</v>
       </c>
     </row>
     <row r="279">
@@ -7153,10 +7153,10 @@
         <v>1084</v>
       </c>
       <c r="H279">
-        <v>42419</v>
+        <v>43398</v>
       </c>
       <c r="I279">
-        <v>3086</v>
+        <v>3143</v>
       </c>
     </row>
     <row r="280">
@@ -7182,10 +7182,10 @@
         <v>1104</v>
       </c>
       <c r="H280">
-        <v>36044</v>
+        <v>35582</v>
       </c>
       <c r="I280">
-        <v>2397</v>
+        <v>2405</v>
       </c>
     </row>
     <row r="281">
@@ -7211,10 +7211,10 @@
         <v>1122</v>
       </c>
       <c r="H281">
-        <v>45270</v>
+        <v>45218</v>
       </c>
       <c r="I281">
-        <v>3262</v>
+        <v>3255</v>
       </c>
     </row>
     <row r="282">
@@ -7240,10 +7240,10 @@
         <v>1148</v>
       </c>
       <c r="H282">
-        <v>46903</v>
+        <v>46798</v>
       </c>
       <c r="I282">
-        <v>2853</v>
+        <v>2857</v>
       </c>
     </row>
     <row r="283">
@@ -7269,7 +7269,7 @@
         <v>1175</v>
       </c>
       <c r="H283">
-        <v>17516</v>
+        <v>17556</v>
       </c>
       <c r="I283">
         <v>1036</v>
@@ -7327,10 +7327,10 @@
         <v>1251</v>
       </c>
       <c r="H285">
-        <v>40950</v>
+        <v>40904</v>
       </c>
       <c r="I285">
-        <v>3441</v>
+        <v>3432</v>
       </c>
     </row>
     <row r="286">
@@ -7356,10 +7356,10 @@
         <v>1309</v>
       </c>
       <c r="H286">
-        <v>55412</v>
+        <v>54313</v>
       </c>
       <c r="I286">
-        <v>4260</v>
+        <v>4255</v>
       </c>
     </row>
     <row r="287">
@@ -7385,10 +7385,10 @@
         <v>1378</v>
       </c>
       <c r="H287">
-        <v>57336</v>
+        <v>57739</v>
       </c>
       <c r="I287">
-        <v>3911</v>
+        <v>3927</v>
       </c>
     </row>
     <row r="288">
@@ -7414,10 +7414,10 @@
         <v>1440</v>
       </c>
       <c r="H288">
-        <v>57178</v>
+        <v>56403</v>
       </c>
       <c r="I288">
-        <v>4008</v>
+        <v>3978</v>
       </c>
     </row>
     <row r="289">
@@ -7443,10 +7443,10 @@
         <v>1510</v>
       </c>
       <c r="H289">
-        <v>64737</v>
+        <v>64626</v>
       </c>
       <c r="I289">
-        <v>3666</v>
+        <v>3700</v>
       </c>
     </row>
     <row r="290">
@@ -7472,10 +7472,10 @@
         <v>1555</v>
       </c>
       <c r="H290">
-        <v>17655</v>
+        <v>17876</v>
       </c>
       <c r="I290">
-        <v>1480</v>
+        <v>1489</v>
       </c>
     </row>
     <row r="291">
@@ -7530,10 +7530,10 @@
         <v>1618</v>
       </c>
       <c r="H292">
-        <v>80874</v>
+        <v>81520</v>
       </c>
       <c r="I292">
-        <v>7159</v>
+        <v>7220</v>
       </c>
     </row>
     <row r="293">
@@ -7559,10 +7559,10 @@
         <v>1686</v>
       </c>
       <c r="H293">
-        <v>82398</v>
+        <v>82467</v>
       </c>
       <c r="I293">
-        <v>5860</v>
+        <v>5846</v>
       </c>
     </row>
     <row r="294">
@@ -7588,10 +7588,10 @@
         <v>1732</v>
       </c>
       <c r="H294">
-        <v>90608</v>
+        <v>91480</v>
       </c>
       <c r="I294">
-        <v>4941</v>
+        <v>5081</v>
       </c>
     </row>
     <row r="295">
@@ -7617,7 +7617,7 @@
         <v>1732</v>
       </c>
       <c r="H295">
-        <v>19252</v>
+        <v>19352</v>
       </c>
       <c r="I295">
         <v>1136</v>
@@ -7675,10 +7675,10 @@
         <v>1773</v>
       </c>
       <c r="H297">
-        <v>2648</v>
+        <v>2278</v>
       </c>
       <c r="I297">
-        <v>232</v>
+        <v>206</v>
       </c>
     </row>
     <row r="298">
@@ -7704,10 +7704,10 @@
         <v>1879</v>
       </c>
       <c r="H298">
-        <v>3092</v>
+        <v>3047</v>
       </c>
       <c r="I298">
-        <v>286</v>
+        <v>280</v>
       </c>
     </row>
     <row r="299">
@@ -7733,10 +7733,10 @@
         <v>1983</v>
       </c>
       <c r="H299">
-        <v>62461</v>
+        <v>63663</v>
       </c>
       <c r="I299">
-        <v>6487</v>
+        <v>6686</v>
       </c>
     </row>
     <row r="300">
@@ -7762,10 +7762,10 @@
         <v>2065</v>
       </c>
       <c r="H300">
-        <v>68069</v>
+        <v>70054</v>
       </c>
       <c r="I300">
-        <v>6628</v>
+        <v>6844</v>
       </c>
     </row>
     <row r="301">
@@ -7791,10 +7791,10 @@
         <v>2138</v>
       </c>
       <c r="H301">
-        <v>64702</v>
+        <v>68737</v>
       </c>
       <c r="I301">
-        <v>5164</v>
+        <v>5426</v>
       </c>
     </row>
     <row r="302">
@@ -7820,10 +7820,10 @@
         <v>2250</v>
       </c>
       <c r="H302">
-        <v>63225</v>
+        <v>71032</v>
       </c>
       <c r="I302">
-        <v>4620</v>
+        <v>5158</v>
       </c>
     </row>
     <row r="303">
@@ -7849,10 +7849,10 @@
         <v>2250</v>
       </c>
       <c r="H303">
-        <v>9566</v>
+        <v>11468</v>
       </c>
       <c r="I303">
-        <v>678</v>
+        <v>753</v>
       </c>
     </row>
     <row r="304">
@@ -7878,10 +7878,10 @@
         <v>2317</v>
       </c>
       <c r="H304">
-        <v>6388</v>
+        <v>6506</v>
       </c>
       <c r="I304">
-        <v>473</v>
+        <v>476</v>
       </c>
     </row>
     <row r="305">
@@ -7907,10 +7907,10 @@
         <v>2521</v>
       </c>
       <c r="H305">
-        <v>3404</v>
+        <v>3077</v>
       </c>
       <c r="I305">
-        <v>312</v>
+        <v>296</v>
       </c>
     </row>
     <row r="306">
@@ -7936,10 +7936,68 @@
         <v>2603</v>
       </c>
       <c r="H306">
-        <v>8676</v>
+        <v>68407</v>
       </c>
       <c r="I306">
-        <v>600</v>
+        <v>6941</v>
+      </c>
+    </row>
+    <row r="307">
+      <c r="A307" s="2">
+        <v>44201</v>
+      </c>
+      <c r="B307">
+        <v>196047</v>
+      </c>
+      <c r="C307">
+        <v>135760</v>
+      </c>
+      <c r="D307">
+        <v>57630</v>
+      </c>
+      <c r="E307">
+        <v>17822</v>
+      </c>
+      <c r="F307">
+        <v>4959</v>
+      </c>
+      <c r="G307">
+        <v>2657</v>
+      </c>
+      <c r="H307">
+        <v>69321</v>
+      </c>
+      <c r="I307">
+        <v>5975</v>
+      </c>
+    </row>
+    <row r="308">
+      <c r="A308" s="2">
+        <v>44202</v>
+      </c>
+      <c r="B308">
+        <v>198184</v>
+      </c>
+      <c r="C308">
+        <v>138383</v>
+      </c>
+      <c r="D308">
+        <v>57084</v>
+      </c>
+      <c r="E308">
+        <v>8257</v>
+      </c>
+      <c r="F308">
+        <v>2137</v>
+      </c>
+      <c r="G308">
+        <v>2717</v>
+      </c>
+      <c r="H308">
+        <v>17028</v>
+      </c>
+      <c r="I308">
+        <v>1424</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated: po 11. 01. 2021
</commit_message>
<xml_diff>
--- a/OpenData_Slovakia_Covid_DailyStats.xlsx
+++ b/OpenData_Slovakia_Covid_DailyStats.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I309"/>
+  <dimension ref="A1:I312"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -7559,7 +7559,7 @@
         <v>1686</v>
       </c>
       <c r="H293">
-        <v>82467</v>
+        <v>82469</v>
       </c>
       <c r="I293">
         <v>5846</v>
@@ -7588,10 +7588,10 @@
         <v>1732</v>
       </c>
       <c r="H294">
-        <v>91485</v>
+        <v>91708</v>
       </c>
       <c r="I294">
-        <v>5081</v>
+        <v>5088</v>
       </c>
     </row>
     <row r="295">
@@ -7733,10 +7733,10 @@
         <v>1983</v>
       </c>
       <c r="H299">
-        <v>63663</v>
+        <v>64720</v>
       </c>
       <c r="I299">
-        <v>6686</v>
+        <v>6798</v>
       </c>
     </row>
     <row r="300">
@@ -7762,10 +7762,10 @@
         <v>2065</v>
       </c>
       <c r="H300">
-        <v>70050</v>
+        <v>70631</v>
       </c>
       <c r="I300">
-        <v>6844</v>
+        <v>6919</v>
       </c>
     </row>
     <row r="301">
@@ -7791,10 +7791,10 @@
         <v>2138</v>
       </c>
       <c r="H301">
-        <v>68742</v>
+        <v>69560</v>
       </c>
       <c r="I301">
-        <v>5427</v>
+        <v>5526</v>
       </c>
     </row>
     <row r="302">
@@ -7820,10 +7820,10 @@
         <v>2250</v>
       </c>
       <c r="H302">
-        <v>71032</v>
+        <v>72518</v>
       </c>
       <c r="I302">
-        <v>5158</v>
+        <v>5281</v>
       </c>
     </row>
     <row r="303">
@@ -7907,10 +7907,10 @@
         <v>2521</v>
       </c>
       <c r="H305">
-        <v>3077</v>
+        <v>3625</v>
       </c>
       <c r="I305">
-        <v>296</v>
+        <v>302</v>
       </c>
     </row>
     <row r="306">
@@ -7936,10 +7936,10 @@
         <v>2603</v>
       </c>
       <c r="H306">
-        <v>68427</v>
+        <v>69879</v>
       </c>
       <c r="I306">
-        <v>6942</v>
+        <v>7112</v>
       </c>
     </row>
     <row r="307">
@@ -7965,10 +7965,10 @@
         <v>2657</v>
       </c>
       <c r="H307">
-        <v>69467</v>
+        <v>72032</v>
       </c>
       <c r="I307">
-        <v>5981</v>
+        <v>6216</v>
       </c>
     </row>
     <row r="308">
@@ -8023,10 +8023,97 @@
         <v>2788</v>
       </c>
       <c r="H309">
-        <v>52845</v>
+        <v>56648</v>
       </c>
       <c r="I309">
-        <v>3626</v>
+        <v>3915</v>
+      </c>
+    </row>
+    <row r="310">
+      <c r="A310" s="2">
+        <v>44204</v>
+      </c>
+      <c r="B310">
+        <v>205236</v>
+      </c>
+      <c r="C310">
+        <v>144612</v>
+      </c>
+      <c r="D310">
+        <v>57788</v>
+      </c>
+      <c r="E310">
+        <v>16368</v>
+      </c>
+      <c r="F310">
+        <v>4072</v>
+      </c>
+      <c r="G310">
+        <v>2836</v>
+      </c>
+      <c r="H310">
+        <v>84945</v>
+      </c>
+      <c r="I310">
+        <v>5131</v>
+      </c>
+    </row>
+    <row r="311">
+      <c r="A311" s="2">
+        <v>44205</v>
+      </c>
+      <c r="B311">
+        <v>208209</v>
+      </c>
+      <c r="C311">
+        <v>147275</v>
+      </c>
+      <c r="D311">
+        <v>58016</v>
+      </c>
+      <c r="E311">
+        <v>12844</v>
+      </c>
+      <c r="F311">
+        <v>2973</v>
+      </c>
+      <c r="G311">
+        <v>2918</v>
+      </c>
+      <c r="H311">
+        <v>22875</v>
+      </c>
+      <c r="I311">
+        <v>1117</v>
+      </c>
+    </row>
+    <row r="312">
+      <c r="A312" s="2">
+        <v>44206</v>
+      </c>
+      <c r="B312">
+        <v>209069</v>
+      </c>
+      <c r="C312">
+        <v>150239</v>
+      </c>
+      <c r="D312">
+        <v>55823</v>
+      </c>
+      <c r="E312">
+        <v>4328</v>
+      </c>
+      <c r="F312">
+        <v>860</v>
+      </c>
+      <c r="G312">
+        <v>3007</v>
+      </c>
+      <c r="H312">
+        <v>31377</v>
+      </c>
+      <c r="I312">
+        <v>1012</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated: st 13. 01. 2021
</commit_message>
<xml_diff>
--- a/OpenData_Slovakia_Covid_DailyStats.xlsx
+++ b/OpenData_Slovakia_Covid_DailyStats.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I313"/>
+  <dimension ref="A1:I314"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -6776,10 +6776,10 @@
         <v>749</v>
       </c>
       <c r="H266">
-        <v>12665</v>
+        <v>12549</v>
       </c>
       <c r="I266">
-        <v>664</v>
+        <v>662</v>
       </c>
     </row>
     <row r="267">
@@ -6805,10 +6805,10 @@
         <v>771</v>
       </c>
       <c r="H267">
-        <v>13318</v>
+        <v>13130</v>
       </c>
       <c r="I267">
-        <v>791</v>
+        <v>779</v>
       </c>
     </row>
     <row r="268">
@@ -6834,10 +6834,10 @@
         <v>798</v>
       </c>
       <c r="H268">
-        <v>14407</v>
+        <v>14021</v>
       </c>
       <c r="I268">
-        <v>697</v>
+        <v>687</v>
       </c>
     </row>
     <row r="269">
@@ -7385,10 +7385,10 @@
         <v>1378</v>
       </c>
       <c r="H287">
-        <v>57739</v>
+        <v>57796</v>
       </c>
       <c r="I287">
-        <v>3927</v>
+        <v>3928</v>
       </c>
     </row>
     <row r="288">
@@ -7414,10 +7414,10 @@
         <v>1440</v>
       </c>
       <c r="H288">
-        <v>56403</v>
+        <v>56583</v>
       </c>
       <c r="I288">
-        <v>3978</v>
+        <v>3990</v>
       </c>
     </row>
     <row r="289">
@@ -7443,10 +7443,10 @@
         <v>1510</v>
       </c>
       <c r="H289">
-        <v>64626</v>
+        <v>64863</v>
       </c>
       <c r="I289">
-        <v>3700</v>
+        <v>3715</v>
       </c>
     </row>
     <row r="290">
@@ -7530,10 +7530,10 @@
         <v>1618</v>
       </c>
       <c r="H292">
-        <v>81522</v>
+        <v>81928</v>
       </c>
       <c r="I292">
-        <v>7220</v>
+        <v>7258</v>
       </c>
     </row>
     <row r="293">
@@ -7559,10 +7559,10 @@
         <v>1686</v>
       </c>
       <c r="H293">
-        <v>82469</v>
+        <v>82860</v>
       </c>
       <c r="I293">
-        <v>5846</v>
+        <v>5859</v>
       </c>
     </row>
     <row r="294">
@@ -7588,10 +7588,10 @@
         <v>1732</v>
       </c>
       <c r="H294">
-        <v>91708</v>
+        <v>92000</v>
       </c>
       <c r="I294">
-        <v>5088</v>
+        <v>5099</v>
       </c>
     </row>
     <row r="295">
@@ -7733,10 +7733,10 @@
         <v>1983</v>
       </c>
       <c r="H299">
-        <v>64720</v>
+        <v>65000</v>
       </c>
       <c r="I299">
-        <v>6798</v>
+        <v>6821</v>
       </c>
     </row>
     <row r="300">
@@ -7762,10 +7762,10 @@
         <v>2065</v>
       </c>
       <c r="H300">
-        <v>70631</v>
+        <v>70834</v>
       </c>
       <c r="I300">
-        <v>6919</v>
+        <v>6930</v>
       </c>
     </row>
     <row r="301">
@@ -7791,10 +7791,10 @@
         <v>2138</v>
       </c>
       <c r="H301">
-        <v>69560</v>
+        <v>69789</v>
       </c>
       <c r="I301">
-        <v>5526</v>
+        <v>5528</v>
       </c>
     </row>
     <row r="302">
@@ -7820,10 +7820,10 @@
         <v>2250</v>
       </c>
       <c r="H302">
-        <v>72518</v>
+        <v>72746</v>
       </c>
       <c r="I302">
-        <v>5281</v>
+        <v>5290</v>
       </c>
     </row>
     <row r="303">
@@ -7936,10 +7936,10 @@
         <v>2603</v>
       </c>
       <c r="H306">
-        <v>70102</v>
+        <v>70319</v>
       </c>
       <c r="I306">
-        <v>7127</v>
+        <v>7147</v>
       </c>
     </row>
     <row r="307">
@@ -7965,10 +7965,10 @@
         <v>2657</v>
       </c>
       <c r="H307">
-        <v>72193</v>
+        <v>72394</v>
       </c>
       <c r="I307">
-        <v>6223</v>
+        <v>6233</v>
       </c>
     </row>
     <row r="308">
@@ -8023,10 +8023,10 @@
         <v>2788</v>
       </c>
       <c r="H309">
-        <v>56421</v>
+        <v>56571</v>
       </c>
       <c r="I309">
-        <v>3906</v>
+        <v>3910</v>
       </c>
     </row>
     <row r="310">
@@ -8052,10 +8052,10 @@
         <v>2836</v>
       </c>
       <c r="H310">
-        <v>86359</v>
+        <v>89093</v>
       </c>
       <c r="I310">
-        <v>5202</v>
+        <v>5333</v>
       </c>
     </row>
     <row r="311">
@@ -8081,10 +8081,10 @@
         <v>2918</v>
       </c>
       <c r="H311">
-        <v>24981</v>
+        <v>32044</v>
       </c>
       <c r="I311">
-        <v>1187</v>
+        <v>1249</v>
       </c>
     </row>
     <row r="312">
@@ -8110,10 +8110,10 @@
         <v>3007</v>
       </c>
       <c r="H312">
-        <v>32901</v>
+        <v>37894</v>
       </c>
       <c r="I312">
-        <v>1058</v>
+        <v>1130</v>
       </c>
     </row>
     <row r="313">
@@ -8139,10 +8139,39 @@
         <v>3102</v>
       </c>
       <c r="H313">
-        <v>67119</v>
+        <v>71472</v>
       </c>
       <c r="I313">
-        <v>3284</v>
+        <v>3450</v>
+      </c>
+    </row>
+    <row r="314">
+      <c r="A314" s="2">
+        <v>44208</v>
+      </c>
+      <c r="B314">
+        <v>215055</v>
+      </c>
+      <c r="C314">
+        <v>157028</v>
+      </c>
+      <c r="D314">
+        <v>54864</v>
+      </c>
+      <c r="E314">
+        <v>15440</v>
+      </c>
+      <c r="F314">
+        <v>3576</v>
+      </c>
+      <c r="G314">
+        <v>3163</v>
+      </c>
+      <c r="H314">
+        <v>62078</v>
+      </c>
+      <c r="I314">
+        <v>3188</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated: pi 15. 01. 2021
</commit_message>
<xml_diff>
--- a/OpenData_Slovakia_Covid_DailyStats.xlsx
+++ b/OpenData_Slovakia_Covid_DailyStats.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I315"/>
+  <dimension ref="A1:I316"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -7356,10 +7356,10 @@
         <v>1309</v>
       </c>
       <c r="H286">
-        <v>54313</v>
+        <v>54344</v>
       </c>
       <c r="I286">
-        <v>4255</v>
+        <v>4260</v>
       </c>
     </row>
     <row r="287">
@@ -7385,10 +7385,10 @@
         <v>1378</v>
       </c>
       <c r="H287">
-        <v>57796</v>
+        <v>57881</v>
       </c>
       <c r="I287">
-        <v>3928</v>
+        <v>3937</v>
       </c>
     </row>
     <row r="288">
@@ -7414,10 +7414,10 @@
         <v>1440</v>
       </c>
       <c r="H288">
-        <v>56583</v>
+        <v>56687</v>
       </c>
       <c r="I288">
-        <v>3990</v>
+        <v>3993</v>
       </c>
     </row>
     <row r="289">
@@ -7443,10 +7443,10 @@
         <v>1510</v>
       </c>
       <c r="H289">
-        <v>65124</v>
+        <v>65263</v>
       </c>
       <c r="I289">
-        <v>3753</v>
+        <v>3764</v>
       </c>
     </row>
     <row r="290">
@@ -7530,10 +7530,10 @@
         <v>1618</v>
       </c>
       <c r="H292">
-        <v>81928</v>
+        <v>82425</v>
       </c>
       <c r="I292">
-        <v>7258</v>
+        <v>7311</v>
       </c>
     </row>
     <row r="293">
@@ -7559,10 +7559,10 @@
         <v>1686</v>
       </c>
       <c r="H293">
-        <v>83032</v>
+        <v>83197</v>
       </c>
       <c r="I293">
-        <v>5864</v>
+        <v>5869</v>
       </c>
     </row>
     <row r="294">
@@ -7588,10 +7588,10 @@
         <v>1732</v>
       </c>
       <c r="H294">
-        <v>92164</v>
+        <v>92254</v>
       </c>
       <c r="I294">
-        <v>5104</v>
+        <v>5110</v>
       </c>
     </row>
     <row r="295">
@@ -7704,10 +7704,10 @@
         <v>1879</v>
       </c>
       <c r="H298">
-        <v>3047</v>
+        <v>3048</v>
       </c>
       <c r="I298">
-        <v>280</v>
+        <v>281</v>
       </c>
     </row>
     <row r="299">
@@ -7733,10 +7733,10 @@
         <v>1983</v>
       </c>
       <c r="H299">
-        <v>65417</v>
+        <v>65636</v>
       </c>
       <c r="I299">
-        <v>6852</v>
+        <v>6884</v>
       </c>
     </row>
     <row r="300">
@@ -7762,10 +7762,10 @@
         <v>2065</v>
       </c>
       <c r="H300">
-        <v>71006</v>
+        <v>71201</v>
       </c>
       <c r="I300">
-        <v>6956</v>
+        <v>6963</v>
       </c>
     </row>
     <row r="301">
@@ -7791,10 +7791,10 @@
         <v>2138</v>
       </c>
       <c r="H301">
-        <v>69975</v>
+        <v>70185</v>
       </c>
       <c r="I301">
-        <v>5553</v>
+        <v>5566</v>
       </c>
     </row>
     <row r="302">
@@ -7820,10 +7820,10 @@
         <v>2250</v>
       </c>
       <c r="H302">
-        <v>73049</v>
+        <v>73183</v>
       </c>
       <c r="I302">
-        <v>5321</v>
+        <v>5336</v>
       </c>
     </row>
     <row r="303">
@@ -7965,10 +7965,10 @@
         <v>2657</v>
       </c>
       <c r="H307">
-        <v>72611</v>
+        <v>73167</v>
       </c>
       <c r="I307">
-        <v>6265</v>
+        <v>6329</v>
       </c>
     </row>
     <row r="308">
@@ -8023,10 +8023,10 @@
         <v>2788</v>
       </c>
       <c r="H309">
-        <v>56861</v>
+        <v>57732</v>
       </c>
       <c r="I309">
-        <v>3950</v>
+        <v>4014</v>
       </c>
     </row>
     <row r="310">
@@ -8052,10 +8052,10 @@
         <v>2836</v>
       </c>
       <c r="H310">
-        <v>89629</v>
+        <v>90050</v>
       </c>
       <c r="I310">
-        <v>5362</v>
+        <v>5389</v>
       </c>
     </row>
     <row r="311">
@@ -8139,10 +8139,10 @@
         <v>3102</v>
       </c>
       <c r="H313">
-        <v>71763</v>
+        <v>72406</v>
       </c>
       <c r="I313">
-        <v>3476</v>
+        <v>3515</v>
       </c>
     </row>
     <row r="314">
@@ -8168,10 +8168,10 @@
         <v>3163</v>
       </c>
       <c r="H314">
-        <v>63716</v>
+        <v>64130</v>
       </c>
       <c r="I314">
-        <v>3279</v>
+        <v>3299</v>
       </c>
     </row>
     <row r="315">
@@ -8197,10 +8197,39 @@
         <v>3260</v>
       </c>
       <c r="H315">
-        <v>63435</v>
+        <v>64594</v>
       </c>
       <c r="I315">
-        <v>2978</v>
+        <v>3034</v>
+      </c>
+    </row>
+    <row r="316">
+      <c r="A316" s="2">
+        <v>44210</v>
+      </c>
+      <c r="B316">
+        <v>220707</v>
+      </c>
+      <c r="C316">
+        <v>163323</v>
+      </c>
+      <c r="D316">
+        <v>54022</v>
+      </c>
+      <c r="E316">
+        <v>11875</v>
+      </c>
+      <c r="F316">
+        <v>2729</v>
+      </c>
+      <c r="G316">
+        <v>3362</v>
+      </c>
+      <c r="H316">
+        <v>46169</v>
+      </c>
+      <c r="I316">
+        <v>2165</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated: po 18. 01. 2021
</commit_message>
<xml_diff>
--- a/OpenData_Slovakia_Covid_DailyStats.xlsx
+++ b/OpenData_Slovakia_Covid_DailyStats.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I316"/>
+  <dimension ref="A1:I319"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -7356,7 +7356,7 @@
         <v>1309</v>
       </c>
       <c r="H286">
-        <v>54344</v>
+        <v>54338</v>
       </c>
       <c r="I286">
         <v>4260</v>
@@ -7385,7 +7385,7 @@
         <v>1378</v>
       </c>
       <c r="H287">
-        <v>57881</v>
+        <v>57852</v>
       </c>
       <c r="I287">
         <v>3937</v>
@@ -7414,10 +7414,10 @@
         <v>1440</v>
       </c>
       <c r="H288">
-        <v>56687</v>
+        <v>56628</v>
       </c>
       <c r="I288">
-        <v>3993</v>
+        <v>3989</v>
       </c>
     </row>
     <row r="289">
@@ -7443,10 +7443,10 @@
         <v>1510</v>
       </c>
       <c r="H289">
-        <v>65263</v>
+        <v>65141</v>
       </c>
       <c r="I289">
-        <v>3764</v>
+        <v>3755</v>
       </c>
     </row>
     <row r="290">
@@ -7530,10 +7530,10 @@
         <v>1618</v>
       </c>
       <c r="H292">
-        <v>82425</v>
+        <v>82191</v>
       </c>
       <c r="I292">
-        <v>7311</v>
+        <v>7298</v>
       </c>
     </row>
     <row r="293">
@@ -7559,10 +7559,10 @@
         <v>1686</v>
       </c>
       <c r="H293">
-        <v>83197</v>
+        <v>82934</v>
       </c>
       <c r="I293">
-        <v>5869</v>
+        <v>5859</v>
       </c>
     </row>
     <row r="294">
@@ -7588,10 +7588,10 @@
         <v>1732</v>
       </c>
       <c r="H294">
-        <v>92254</v>
+        <v>92249</v>
       </c>
       <c r="I294">
-        <v>5110</v>
+        <v>5106</v>
       </c>
     </row>
     <row r="295">
@@ -7733,10 +7733,10 @@
         <v>1983</v>
       </c>
       <c r="H299">
-        <v>65636</v>
+        <v>65331</v>
       </c>
       <c r="I299">
-        <v>6884</v>
+        <v>6841</v>
       </c>
     </row>
     <row r="300">
@@ -7762,10 +7762,10 @@
         <v>2065</v>
       </c>
       <c r="H300">
-        <v>71201</v>
+        <v>70987</v>
       </c>
       <c r="I300">
-        <v>6963</v>
+        <v>6949</v>
       </c>
     </row>
     <row r="301">
@@ -7791,10 +7791,10 @@
         <v>2138</v>
       </c>
       <c r="H301">
-        <v>70185</v>
+        <v>70116</v>
       </c>
       <c r="I301">
-        <v>5566</v>
+        <v>5571</v>
       </c>
     </row>
     <row r="302">
@@ -7820,10 +7820,10 @@
         <v>2250</v>
       </c>
       <c r="H302">
-        <v>73183</v>
+        <v>72962</v>
       </c>
       <c r="I302">
-        <v>5336</v>
+        <v>5329</v>
       </c>
     </row>
     <row r="303">
@@ -7936,10 +7936,10 @@
         <v>2603</v>
       </c>
       <c r="H306">
-        <v>70612</v>
+        <v>70279</v>
       </c>
       <c r="I306">
-        <v>7170</v>
+        <v>7150</v>
       </c>
     </row>
     <row r="307">
@@ -7965,10 +7965,10 @@
         <v>2657</v>
       </c>
       <c r="H307">
-        <v>73167</v>
+        <v>73273</v>
       </c>
       <c r="I307">
-        <v>6329</v>
+        <v>6338</v>
       </c>
     </row>
     <row r="308">
@@ -7994,10 +7994,10 @@
         <v>2717</v>
       </c>
       <c r="H308">
-        <v>17036</v>
+        <v>17044</v>
       </c>
       <c r="I308">
-        <v>1424</v>
+        <v>1425</v>
       </c>
     </row>
     <row r="309">
@@ -8023,10 +8023,10 @@
         <v>2788</v>
       </c>
       <c r="H309">
-        <v>57732</v>
+        <v>57500</v>
       </c>
       <c r="I309">
-        <v>4014</v>
+        <v>3996</v>
       </c>
     </row>
     <row r="310">
@@ -8052,10 +8052,10 @@
         <v>2836</v>
       </c>
       <c r="H310">
-        <v>90050</v>
+        <v>90010</v>
       </c>
       <c r="I310">
-        <v>5389</v>
+        <v>5382</v>
       </c>
     </row>
     <row r="311">
@@ -8139,10 +8139,10 @@
         <v>3102</v>
       </c>
       <c r="H313">
-        <v>72406</v>
+        <v>72877</v>
       </c>
       <c r="I313">
-        <v>3515</v>
+        <v>3546</v>
       </c>
     </row>
     <row r="314">
@@ -8168,10 +8168,10 @@
         <v>3163</v>
       </c>
       <c r="H314">
-        <v>64130</v>
+        <v>64970</v>
       </c>
       <c r="I314">
-        <v>3299</v>
+        <v>3344</v>
       </c>
     </row>
     <row r="315">
@@ -8197,10 +8197,10 @@
         <v>3260</v>
       </c>
       <c r="H315">
-        <v>64594</v>
+        <v>65840</v>
       </c>
       <c r="I315">
-        <v>3034</v>
+        <v>3095</v>
       </c>
     </row>
     <row r="316">
@@ -8226,10 +8226,97 @@
         <v>3362</v>
       </c>
       <c r="H316">
-        <v>46169</v>
+        <v>49427</v>
       </c>
       <c r="I316">
-        <v>2165</v>
+        <v>2300</v>
+      </c>
+    </row>
+    <row r="317">
+      <c r="A317" s="2">
+        <v>44211</v>
+      </c>
+      <c r="B317">
+        <v>222752</v>
+      </c>
+      <c r="C317">
+        <v>166555</v>
+      </c>
+      <c r="D317">
+        <v>52780</v>
+      </c>
+      <c r="E317">
+        <v>11392</v>
+      </c>
+      <c r="F317">
+        <v>2045</v>
+      </c>
+      <c r="G317">
+        <v>3417</v>
+      </c>
+      <c r="H317">
+        <v>58918</v>
+      </c>
+      <c r="I317">
+        <v>2079</v>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" s="2">
+        <v>44212</v>
+      </c>
+      <c r="B318">
+        <v>223325</v>
+      </c>
+      <c r="C318">
+        <v>168915</v>
+      </c>
+      <c r="D318">
+        <v>50936</v>
+      </c>
+      <c r="E318">
+        <v>2850</v>
+      </c>
+      <c r="F318">
+        <v>573</v>
+      </c>
+      <c r="G318">
+        <v>3474</v>
+      </c>
+      <c r="H318">
+        <v>19705</v>
+      </c>
+      <c r="I318">
+        <v>783</v>
+      </c>
+    </row>
+    <row r="319">
+      <c r="A319" s="2">
+        <v>44213</v>
+      </c>
+      <c r="B319">
+        <v>224385</v>
+      </c>
+      <c r="C319">
+        <v>171092</v>
+      </c>
+      <c r="D319">
+        <v>49767</v>
+      </c>
+      <c r="E319">
+        <v>6252</v>
+      </c>
+      <c r="F319">
+        <v>1060</v>
+      </c>
+      <c r="G319">
+        <v>3526</v>
+      </c>
+      <c r="H319">
+        <v>37771</v>
+      </c>
+      <c r="I319">
+        <v>676</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated: ut 19. 01. 2021
</commit_message>
<xml_diff>
--- a/OpenData_Slovakia_Covid_DailyStats.xlsx
+++ b/OpenData_Slovakia_Covid_DailyStats.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I319"/>
+  <dimension ref="A1:I320"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -7733,7 +7733,7 @@
         <v>1983</v>
       </c>
       <c r="H299">
-        <v>65331</v>
+        <v>65337</v>
       </c>
       <c r="I299">
         <v>6841</v>
@@ -8052,10 +8052,10 @@
         <v>2836</v>
       </c>
       <c r="H310">
-        <v>90010</v>
+        <v>90228</v>
       </c>
       <c r="I310">
-        <v>5382</v>
+        <v>5391</v>
       </c>
     </row>
     <row r="311">
@@ -8139,10 +8139,10 @@
         <v>3102</v>
       </c>
       <c r="H313">
-        <v>72877</v>
+        <v>73035</v>
       </c>
       <c r="I313">
-        <v>3546</v>
+        <v>3559</v>
       </c>
     </row>
     <row r="314">
@@ -8168,7 +8168,7 @@
         <v>3163</v>
       </c>
       <c r="H314">
-        <v>64970</v>
+        <v>64976</v>
       </c>
       <c r="I314">
         <v>3344</v>
@@ -8197,10 +8197,10 @@
         <v>3260</v>
       </c>
       <c r="H315">
-        <v>65840</v>
+        <v>65955</v>
       </c>
       <c r="I315">
-        <v>3095</v>
+        <v>3104</v>
       </c>
     </row>
     <row r="316">
@@ -8226,10 +8226,10 @@
         <v>3362</v>
       </c>
       <c r="H316">
-        <v>49427</v>
+        <v>49034</v>
       </c>
       <c r="I316">
-        <v>2300</v>
+        <v>2278</v>
       </c>
     </row>
     <row r="317">
@@ -8255,10 +8255,10 @@
         <v>3417</v>
       </c>
       <c r="H317">
-        <v>58918</v>
+        <v>60995</v>
       </c>
       <c r="I317">
-        <v>2079</v>
+        <v>2119</v>
       </c>
     </row>
     <row r="318">
@@ -8284,10 +8284,10 @@
         <v>3474</v>
       </c>
       <c r="H318">
-        <v>19705</v>
+        <v>24466</v>
       </c>
       <c r="I318">
-        <v>783</v>
+        <v>875</v>
       </c>
     </row>
     <row r="319">
@@ -8313,10 +8313,39 @@
         <v>3526</v>
       </c>
       <c r="H319">
-        <v>37771</v>
+        <v>40781</v>
       </c>
       <c r="I319">
-        <v>676</v>
+        <v>783</v>
+      </c>
+    </row>
+    <row r="320">
+      <c r="A320" s="2">
+        <v>44214</v>
+      </c>
+      <c r="B320">
+        <v>226294</v>
+      </c>
+      <c r="C320">
+        <v>173761</v>
+      </c>
+      <c r="D320">
+        <v>48896</v>
+      </c>
+      <c r="E320">
+        <v>9817</v>
+      </c>
+      <c r="F320">
+        <v>1909</v>
+      </c>
+      <c r="G320">
+        <v>3637</v>
+      </c>
+      <c r="H320">
+        <v>83214</v>
+      </c>
+      <c r="I320">
+        <v>4046</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated: št 21. 01. 2021
</commit_message>
<xml_diff>
--- a/OpenData_Slovakia_Covid_DailyStats.xlsx
+++ b/OpenData_Slovakia_Covid_DailyStats.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I321"/>
+  <dimension ref="A1:I322"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -7356,10 +7356,10 @@
         <v>1309</v>
       </c>
       <c r="H286">
-        <v>54338</v>
+        <v>54215</v>
       </c>
       <c r="I286">
-        <v>4260</v>
+        <v>4250</v>
       </c>
     </row>
     <row r="287">
@@ -7385,10 +7385,10 @@
         <v>1378</v>
       </c>
       <c r="H287">
-        <v>57852</v>
+        <v>57631</v>
       </c>
       <c r="I287">
-        <v>3937</v>
+        <v>3917</v>
       </c>
     </row>
     <row r="288">
@@ -7414,10 +7414,10 @@
         <v>1440</v>
       </c>
       <c r="H288">
-        <v>56628</v>
+        <v>56088</v>
       </c>
       <c r="I288">
-        <v>3989</v>
+        <v>3959</v>
       </c>
     </row>
     <row r="289">
@@ -7443,10 +7443,10 @@
         <v>1510</v>
       </c>
       <c r="H289">
-        <v>65141</v>
+        <v>64387</v>
       </c>
       <c r="I289">
-        <v>3755</v>
+        <v>3698</v>
       </c>
     </row>
     <row r="290">
@@ -7530,10 +7530,10 @@
         <v>1618</v>
       </c>
       <c r="H292">
-        <v>82191</v>
+        <v>81217</v>
       </c>
       <c r="I292">
-        <v>7298</v>
+        <v>7191</v>
       </c>
     </row>
     <row r="293">
@@ -7559,10 +7559,10 @@
         <v>1686</v>
       </c>
       <c r="H293">
-        <v>82934</v>
+        <v>81670</v>
       </c>
       <c r="I293">
-        <v>5859</v>
+        <v>5794</v>
       </c>
     </row>
     <row r="294">
@@ -7588,10 +7588,10 @@
         <v>1732</v>
       </c>
       <c r="H294">
-        <v>92249</v>
+        <v>90791</v>
       </c>
       <c r="I294">
-        <v>5106</v>
+        <v>5028</v>
       </c>
     </row>
     <row r="295">
@@ -7675,10 +7675,10 @@
         <v>1773</v>
       </c>
       <c r="H297">
-        <v>2278</v>
+        <v>2282</v>
       </c>
       <c r="I297">
-        <v>206</v>
+        <v>208</v>
       </c>
     </row>
     <row r="298">
@@ -7733,10 +7733,10 @@
         <v>1983</v>
       </c>
       <c r="H299">
-        <v>65337</v>
+        <v>63795</v>
       </c>
       <c r="I299">
-        <v>6841</v>
+        <v>6698</v>
       </c>
     </row>
     <row r="300">
@@ -7762,10 +7762,10 @@
         <v>2065</v>
       </c>
       <c r="H300">
-        <v>70987</v>
+        <v>70477</v>
       </c>
       <c r="I300">
-        <v>6949</v>
+        <v>6917</v>
       </c>
     </row>
     <row r="301">
@@ -7791,10 +7791,10 @@
         <v>2138</v>
       </c>
       <c r="H301">
-        <v>70116</v>
+        <v>69571</v>
       </c>
       <c r="I301">
-        <v>5571</v>
+        <v>5560</v>
       </c>
     </row>
     <row r="302">
@@ -7820,10 +7820,10 @@
         <v>2250</v>
       </c>
       <c r="H302">
-        <v>72962</v>
+        <v>72559</v>
       </c>
       <c r="I302">
-        <v>5329</v>
+        <v>5284</v>
       </c>
     </row>
     <row r="303">
@@ -7936,10 +7936,10 @@
         <v>2603</v>
       </c>
       <c r="H306">
-        <v>70279</v>
+        <v>70727</v>
       </c>
       <c r="I306">
-        <v>7150</v>
+        <v>7182</v>
       </c>
     </row>
     <row r="307">
@@ -7965,10 +7965,10 @@
         <v>2657</v>
       </c>
       <c r="H307">
-        <v>73273</v>
+        <v>73350</v>
       </c>
       <c r="I307">
-        <v>6338</v>
+        <v>6323</v>
       </c>
     </row>
     <row r="308">
@@ -8023,10 +8023,10 @@
         <v>2788</v>
       </c>
       <c r="H309">
-        <v>57500</v>
+        <v>57091</v>
       </c>
       <c r="I309">
-        <v>3996</v>
+        <v>3950</v>
       </c>
     </row>
     <row r="310">
@@ -8052,10 +8052,10 @@
         <v>2836</v>
       </c>
       <c r="H310">
-        <v>90228</v>
+        <v>90811</v>
       </c>
       <c r="I310">
-        <v>5391</v>
+        <v>5414</v>
       </c>
     </row>
     <row r="311">
@@ -8139,10 +8139,10 @@
         <v>3102</v>
       </c>
       <c r="H313">
-        <v>73039</v>
+        <v>72895</v>
       </c>
       <c r="I313">
-        <v>3559</v>
+        <v>3546</v>
       </c>
     </row>
     <row r="314">
@@ -8168,10 +8168,10 @@
         <v>3163</v>
       </c>
       <c r="H314">
-        <v>64984</v>
+        <v>65072</v>
       </c>
       <c r="I314">
-        <v>3344</v>
+        <v>3346</v>
       </c>
     </row>
     <row r="315">
@@ -8197,10 +8197,10 @@
         <v>3260</v>
       </c>
       <c r="H315">
-        <v>65958</v>
+        <v>65997</v>
       </c>
       <c r="I315">
-        <v>3104</v>
+        <v>3106</v>
       </c>
     </row>
     <row r="316">
@@ -8226,7 +8226,7 @@
         <v>3362</v>
       </c>
       <c r="H316">
-        <v>49036</v>
+        <v>49041</v>
       </c>
       <c r="I316">
         <v>2278</v>
@@ -8255,7 +8255,7 @@
         <v>3417</v>
       </c>
       <c r="H317">
-        <v>61017</v>
+        <v>61020</v>
       </c>
       <c r="I317">
         <v>2122</v>
@@ -8342,10 +8342,10 @@
         <v>3637</v>
       </c>
       <c r="H320">
-        <v>83190</v>
+        <v>83674</v>
       </c>
       <c r="I320">
-        <v>4060</v>
+        <v>4065</v>
       </c>
     </row>
     <row r="321">
@@ -8371,10 +8371,39 @@
         <v>3737</v>
       </c>
       <c r="H321">
-        <v>33082</v>
+        <v>80975</v>
       </c>
       <c r="I321">
-        <v>1325</v>
+        <v>2654</v>
+      </c>
+    </row>
+    <row r="322">
+      <c r="A322" s="2">
+        <v>44216</v>
+      </c>
+      <c r="B322">
+        <v>231242</v>
+      </c>
+      <c r="C322">
+        <v>181129</v>
+      </c>
+      <c r="D322">
+        <v>46312</v>
+      </c>
+      <c r="E322">
+        <v>12668</v>
+      </c>
+      <c r="F322">
+        <v>2464</v>
+      </c>
+      <c r="G322">
+        <v>3801</v>
+      </c>
+      <c r="H322">
+        <v>82510</v>
+      </c>
+      <c r="I322">
+        <v>2045</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated: pi 22. 01. 2021
</commit_message>
<xml_diff>
--- a/OpenData_Slovakia_Covid_DailyStats.xlsx
+++ b/OpenData_Slovakia_Covid_DailyStats.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I322"/>
+  <dimension ref="A1:I323"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -8023,7 +8023,7 @@
         <v>2788</v>
       </c>
       <c r="H309">
-        <v>57091</v>
+        <v>57096</v>
       </c>
       <c r="I309">
         <v>3950</v>
@@ -8081,10 +8081,10 @@
         <v>2918</v>
       </c>
       <c r="H311">
-        <v>37383</v>
+        <v>37385</v>
       </c>
       <c r="I311">
-        <v>1400</v>
+        <v>1401</v>
       </c>
     </row>
     <row r="312">
@@ -8342,7 +8342,7 @@
         <v>3637</v>
       </c>
       <c r="H320">
-        <v>83674</v>
+        <v>83763</v>
       </c>
       <c r="I320">
         <v>4065</v>
@@ -8371,10 +8371,10 @@
         <v>3737</v>
       </c>
       <c r="H321">
-        <v>80975</v>
+        <v>84133</v>
       </c>
       <c r="I321">
-        <v>2654</v>
+        <v>2636</v>
       </c>
     </row>
     <row r="322">
@@ -8400,10 +8400,39 @@
         <v>3801</v>
       </c>
       <c r="H322">
-        <v>82510</v>
+        <v>98715</v>
       </c>
       <c r="I322">
-        <v>2045</v>
+        <v>2208</v>
+      </c>
+    </row>
+    <row r="323">
+      <c r="A323" s="2">
+        <v>44217</v>
+      </c>
+      <c r="B323">
+        <v>233027</v>
+      </c>
+      <c r="C323">
+        <v>183942</v>
+      </c>
+      <c r="D323">
+        <v>45191</v>
+      </c>
+      <c r="E323">
+        <v>11018</v>
+      </c>
+      <c r="F323">
+        <v>1785</v>
+      </c>
+      <c r="G323">
+        <v>3894</v>
+      </c>
+      <c r="H323">
+        <v>127818</v>
+      </c>
+      <c r="I323">
+        <v>1999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated: so 23. 01. 2021
</commit_message>
<xml_diff>
--- a/OpenData_Slovakia_Covid_DailyStats.xlsx
+++ b/OpenData_Slovakia_Covid_DailyStats.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I323"/>
+  <dimension ref="A1:I324"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -5529,7 +5529,7 @@
         <v>66</v>
       </c>
       <c r="H223">
-        <v>1155</v>
+        <v>1152</v>
       </c>
       <c r="I223">
         <v>84</v>
@@ -5732,7 +5732,7 @@
         <v>98</v>
       </c>
       <c r="H230">
-        <v>613</v>
+        <v>614</v>
       </c>
       <c r="I230">
         <v>38</v>
@@ -5790,7 +5790,7 @@
         <v>134</v>
       </c>
       <c r="H232">
-        <v>2136</v>
+        <v>2138</v>
       </c>
       <c r="I232">
         <v>141</v>
@@ -5993,7 +5993,7 @@
         <v>212</v>
       </c>
       <c r="H239">
-        <v>6149</v>
+        <v>6185</v>
       </c>
       <c r="I239">
         <v>239</v>
@@ -6022,7 +6022,7 @@
         <v>219</v>
       </c>
       <c r="H240">
-        <v>41133</v>
+        <v>41132</v>
       </c>
       <c r="I240">
         <v>471</v>
@@ -6167,7 +6167,7 @@
         <v>286</v>
       </c>
       <c r="H245">
-        <v>3592</v>
+        <v>3596</v>
       </c>
       <c r="I245">
         <v>82</v>
@@ -6196,7 +6196,7 @@
         <v>317</v>
       </c>
       <c r="H246">
-        <v>2115</v>
+        <v>2114</v>
       </c>
       <c r="I246">
         <v>140</v>
@@ -6254,7 +6254,7 @@
         <v>351</v>
       </c>
       <c r="H248">
-        <v>45190</v>
+        <v>45188</v>
       </c>
       <c r="I248">
         <v>439</v>
@@ -6399,7 +6399,7 @@
         <v>491</v>
       </c>
       <c r="H253">
-        <v>5606</v>
+        <v>5636</v>
       </c>
       <c r="I253">
         <v>173</v>
@@ -6428,7 +6428,7 @@
         <v>510</v>
       </c>
       <c r="H254">
-        <v>6144</v>
+        <v>6145</v>
       </c>
       <c r="I254">
         <v>158</v>
@@ -6486,7 +6486,7 @@
         <v>526</v>
       </c>
       <c r="H256">
-        <v>1242</v>
+        <v>1245</v>
       </c>
       <c r="I256">
         <v>33</v>
@@ -6544,7 +6544,7 @@
         <v>579</v>
       </c>
       <c r="H258">
-        <v>3860</v>
+        <v>3859</v>
       </c>
       <c r="I258">
         <v>218</v>
@@ -6573,7 +6573,7 @@
         <v>579</v>
       </c>
       <c r="H259">
-        <v>6103</v>
+        <v>6104</v>
       </c>
       <c r="I259">
         <v>419</v>
@@ -6602,7 +6602,7 @@
         <v>614</v>
       </c>
       <c r="H260">
-        <v>11479</v>
+        <v>11611</v>
       </c>
       <c r="I260">
         <v>746</v>
@@ -6805,7 +6805,7 @@
         <v>771</v>
       </c>
       <c r="H267">
-        <v>13130</v>
+        <v>13242</v>
       </c>
       <c r="I267">
         <v>779</v>
@@ -6921,7 +6921,7 @@
         <v>868</v>
       </c>
       <c r="H271">
-        <v>42580</v>
+        <v>42584</v>
       </c>
       <c r="I271">
         <v>1620</v>
@@ -7037,7 +7037,7 @@
         <v>981</v>
       </c>
       <c r="H275">
-        <v>28740</v>
+        <v>28741</v>
       </c>
       <c r="I275">
         <v>1239</v>
@@ -7124,7 +7124,7 @@
         <v>1046</v>
       </c>
       <c r="H278">
-        <v>29996</v>
+        <v>30001</v>
       </c>
       <c r="I278">
         <v>2101</v>
@@ -7153,7 +7153,7 @@
         <v>1084</v>
       </c>
       <c r="H279">
-        <v>43398</v>
+        <v>43382</v>
       </c>
       <c r="I279">
         <v>3143</v>
@@ -7182,7 +7182,7 @@
         <v>1104</v>
       </c>
       <c r="H280">
-        <v>35582</v>
+        <v>35570</v>
       </c>
       <c r="I280">
         <v>2405</v>
@@ -7211,7 +7211,7 @@
         <v>1122</v>
       </c>
       <c r="H281">
-        <v>45218</v>
+        <v>45201</v>
       </c>
       <c r="I281">
         <v>3255</v>
@@ -7240,7 +7240,7 @@
         <v>1148</v>
       </c>
       <c r="H282">
-        <v>46798</v>
+        <v>46781</v>
       </c>
       <c r="I282">
         <v>2857</v>
@@ -7327,7 +7327,7 @@
         <v>1251</v>
       </c>
       <c r="H285">
-        <v>40904</v>
+        <v>40884</v>
       </c>
       <c r="I285">
         <v>3432</v>
@@ -7356,7 +7356,7 @@
         <v>1309</v>
       </c>
       <c r="H286">
-        <v>54215</v>
+        <v>54196</v>
       </c>
       <c r="I286">
         <v>4250</v>
@@ -7385,7 +7385,7 @@
         <v>1378</v>
       </c>
       <c r="H287">
-        <v>57631</v>
+        <v>57619</v>
       </c>
       <c r="I287">
         <v>3917</v>
@@ -7414,7 +7414,7 @@
         <v>1440</v>
       </c>
       <c r="H288">
-        <v>56088</v>
+        <v>56086</v>
       </c>
       <c r="I288">
         <v>3959</v>
@@ -7443,7 +7443,7 @@
         <v>1510</v>
       </c>
       <c r="H289">
-        <v>64387</v>
+        <v>64384</v>
       </c>
       <c r="I289">
         <v>3698</v>
@@ -7501,7 +7501,7 @@
         <v>1618</v>
       </c>
       <c r="H291">
-        <v>14826</v>
+        <v>14831</v>
       </c>
       <c r="I291">
         <v>483</v>
@@ -7530,7 +7530,7 @@
         <v>1618</v>
       </c>
       <c r="H292">
-        <v>81217</v>
+        <v>81212</v>
       </c>
       <c r="I292">
         <v>7191</v>
@@ -7559,7 +7559,7 @@
         <v>1686</v>
       </c>
       <c r="H293">
-        <v>81670</v>
+        <v>81666</v>
       </c>
       <c r="I293">
         <v>5794</v>
@@ -7588,7 +7588,7 @@
         <v>1732</v>
       </c>
       <c r="H294">
-        <v>90791</v>
+        <v>90790</v>
       </c>
       <c r="I294">
         <v>5028</v>
@@ -7617,7 +7617,7 @@
         <v>1732</v>
       </c>
       <c r="H295">
-        <v>19352</v>
+        <v>19353</v>
       </c>
       <c r="I295">
         <v>1136</v>
@@ -7762,7 +7762,7 @@
         <v>2065</v>
       </c>
       <c r="H300">
-        <v>70477</v>
+        <v>70476</v>
       </c>
       <c r="I300">
         <v>6917</v>
@@ -7820,7 +7820,7 @@
         <v>2250</v>
       </c>
       <c r="H302">
-        <v>72559</v>
+        <v>72555</v>
       </c>
       <c r="I302">
         <v>5284</v>
@@ -7936,7 +7936,7 @@
         <v>2603</v>
       </c>
       <c r="H306">
-        <v>70727</v>
+        <v>70725</v>
       </c>
       <c r="I306">
         <v>7182</v>
@@ -7965,7 +7965,7 @@
         <v>2657</v>
       </c>
       <c r="H307">
-        <v>73350</v>
+        <v>73347</v>
       </c>
       <c r="I307">
         <v>6323</v>
@@ -8023,7 +8023,7 @@
         <v>2788</v>
       </c>
       <c r="H309">
-        <v>57096</v>
+        <v>57092</v>
       </c>
       <c r="I309">
         <v>3950</v>
@@ -8052,7 +8052,7 @@
         <v>2836</v>
       </c>
       <c r="H310">
-        <v>90811</v>
+        <v>90810</v>
       </c>
       <c r="I310">
         <v>5414</v>
@@ -8139,7 +8139,7 @@
         <v>3102</v>
       </c>
       <c r="H313">
-        <v>72895</v>
+        <v>72891</v>
       </c>
       <c r="I313">
         <v>3546</v>
@@ -8168,7 +8168,7 @@
         <v>3163</v>
       </c>
       <c r="H314">
-        <v>65072</v>
+        <v>65070</v>
       </c>
       <c r="I314">
         <v>3346</v>
@@ -8226,7 +8226,7 @@
         <v>3362</v>
       </c>
       <c r="H316">
-        <v>49041</v>
+        <v>49040</v>
       </c>
       <c r="I316">
         <v>2278</v>
@@ -8284,7 +8284,7 @@
         <v>3474</v>
       </c>
       <c r="H318">
-        <v>24466</v>
+        <v>24467</v>
       </c>
       <c r="I318">
         <v>875</v>
@@ -8342,7 +8342,7 @@
         <v>3637</v>
       </c>
       <c r="H320">
-        <v>83763</v>
+        <v>83746</v>
       </c>
       <c r="I320">
         <v>4065</v>
@@ -8400,7 +8400,7 @@
         <v>3801</v>
       </c>
       <c r="H322">
-        <v>98715</v>
+        <v>98713</v>
       </c>
       <c r="I322">
         <v>2208</v>
@@ -8433,6 +8433,35 @@
       </c>
       <c r="I323">
         <v>1999</v>
+      </c>
+    </row>
+    <row r="324">
+      <c r="A324" s="2">
+        <v>44218</v>
+      </c>
+      <c r="B324">
+        <v>50063</v>
+      </c>
+      <c r="C324">
+        <v>186683</v>
+      </c>
+      <c r="D324">
+        <v>-140585</v>
+      </c>
+      <c r="E324">
+        <v>20264</v>
+      </c>
+      <c r="F324">
+        <v>-182964</v>
+      </c>
+      <c r="G324">
+        <v>3965</v>
+      </c>
+      <c r="H324">
+        <v>30746</v>
+      </c>
+      <c r="I324">
+        <v>437</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated: po 25. 01. 2021
</commit_message>
<xml_diff>
--- a/OpenData_Slovakia_Covid_DailyStats.xlsx
+++ b/OpenData_Slovakia_Covid_DailyStats.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I324"/>
+  <dimension ref="A1:I326"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -7530,7 +7530,7 @@
         <v>1618</v>
       </c>
       <c r="H292">
-        <v>81212</v>
+        <v>81215</v>
       </c>
       <c r="I292">
         <v>7191</v>
@@ -7936,7 +7936,7 @@
         <v>2603</v>
       </c>
       <c r="H306">
-        <v>70725</v>
+        <v>70727</v>
       </c>
       <c r="I306">
         <v>7182</v>
@@ -8023,10 +8023,10 @@
         <v>2788</v>
       </c>
       <c r="H309">
-        <v>57092</v>
+        <v>57318</v>
       </c>
       <c r="I309">
-        <v>3950</v>
+        <v>3964</v>
       </c>
     </row>
     <row r="310">
@@ -8197,10 +8197,10 @@
         <v>3260</v>
       </c>
       <c r="H315">
-        <v>65997</v>
+        <v>66051</v>
       </c>
       <c r="I315">
-        <v>3106</v>
+        <v>3010</v>
       </c>
     </row>
     <row r="316">
@@ -8255,10 +8255,10 @@
         <v>3417</v>
       </c>
       <c r="H317">
-        <v>61020</v>
+        <v>61022</v>
       </c>
       <c r="I317">
-        <v>2122</v>
+        <v>2124</v>
       </c>
     </row>
     <row r="318">
@@ -8284,10 +8284,10 @@
         <v>3474</v>
       </c>
       <c r="H318">
-        <v>24467</v>
+        <v>24692</v>
       </c>
       <c r="I318">
-        <v>875</v>
+        <v>888</v>
       </c>
     </row>
     <row r="319">
@@ -8342,10 +8342,10 @@
         <v>3637</v>
       </c>
       <c r="H320">
-        <v>83746</v>
+        <v>86035</v>
       </c>
       <c r="I320">
-        <v>4065</v>
+        <v>4194</v>
       </c>
     </row>
     <row r="321">
@@ -8371,10 +8371,10 @@
         <v>3737</v>
       </c>
       <c r="H321">
-        <v>84133</v>
+        <v>86604</v>
       </c>
       <c r="I321">
-        <v>2636</v>
+        <v>2686</v>
       </c>
     </row>
     <row r="322">
@@ -8400,10 +8400,10 @@
         <v>3801</v>
       </c>
       <c r="H322">
-        <v>98713</v>
+        <v>102224</v>
       </c>
       <c r="I322">
-        <v>2208</v>
+        <v>2255</v>
       </c>
     </row>
     <row r="323">
@@ -8429,10 +8429,10 @@
         <v>3894</v>
       </c>
       <c r="H323">
-        <v>127818</v>
+        <v>143426</v>
       </c>
       <c r="I323">
-        <v>1999</v>
+        <v>2235</v>
       </c>
     </row>
     <row r="324">
@@ -8440,28 +8440,86 @@
         <v>44218</v>
       </c>
       <c r="B324">
-        <v>50063</v>
+        <v>234571</v>
       </c>
       <c r="C324">
         <v>186683</v>
       </c>
       <c r="D324">
-        <v>-140585</v>
+        <v>43923</v>
       </c>
       <c r="E324">
         <v>20264</v>
       </c>
       <c r="F324">
-        <v>-182964</v>
+        <v>1544</v>
       </c>
       <c r="G324">
         <v>3965</v>
       </c>
       <c r="H324">
-        <v>30746</v>
+        <v>209823</v>
       </c>
       <c r="I324">
-        <v>437</v>
+        <v>2458</v>
+      </c>
+    </row>
+    <row r="325">
+      <c r="A325" s="2">
+        <v>44219</v>
+      </c>
+      <c r="B325">
+        <v>236476</v>
+      </c>
+      <c r="C325">
+        <v>189959</v>
+      </c>
+      <c r="D325">
+        <v>42449</v>
+      </c>
+      <c r="E325">
+        <v>16498</v>
+      </c>
+      <c r="F325">
+        <v>1905</v>
+      </c>
+      <c r="G325">
+        <v>4068</v>
+      </c>
+      <c r="H325">
+        <v>562488</v>
+      </c>
+      <c r="I325">
+        <v>5346</v>
+      </c>
+    </row>
+    <row r="326">
+      <c r="A326" s="2">
+        <v>44220</v>
+      </c>
+      <c r="B326">
+        <v>237027</v>
+      </c>
+      <c r="C326">
+        <v>193380</v>
+      </c>
+      <c r="D326">
+        <v>39579</v>
+      </c>
+      <c r="E326">
+        <v>3806</v>
+      </c>
+      <c r="F326">
+        <v>551</v>
+      </c>
+      <c r="G326">
+        <v>4068</v>
+      </c>
+      <c r="H326">
+        <v>284768</v>
+      </c>
+      <c r="I326">
+        <v>2322</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated: ut 26. 01. 2021
</commit_message>
<xml_diff>
--- a/OpenData_Slovakia_Covid_DailyStats.xlsx
+++ b/OpenData_Slovakia_Covid_DailyStats.xlsx
@@ -7443,10 +7443,10 @@
         <v>1510</v>
       </c>
       <c r="H289">
-        <v>64384</v>
+        <v>64395</v>
       </c>
       <c r="I289">
-        <v>3698</v>
+        <v>3699</v>
       </c>
     </row>
     <row r="290">
@@ -7530,7 +7530,7 @@
         <v>1618</v>
       </c>
       <c r="H292">
-        <v>81215</v>
+        <v>81241</v>
       </c>
       <c r="I292">
         <v>7191</v>
@@ -7733,10 +7733,10 @@
         <v>1983</v>
       </c>
       <c r="H299">
-        <v>63795</v>
+        <v>64055</v>
       </c>
       <c r="I299">
-        <v>6698</v>
+        <v>6713</v>
       </c>
     </row>
     <row r="300">
@@ -7936,7 +7936,7 @@
         <v>2603</v>
       </c>
       <c r="H306">
-        <v>70727</v>
+        <v>70729</v>
       </c>
       <c r="I306">
         <v>7182</v>
@@ -8023,10 +8023,10 @@
         <v>2788</v>
       </c>
       <c r="H309">
-        <v>57318</v>
+        <v>57315</v>
       </c>
       <c r="I309">
-        <v>3964</v>
+        <v>3962</v>
       </c>
     </row>
     <row r="310">
@@ -8052,10 +8052,10 @@
         <v>2836</v>
       </c>
       <c r="H310">
-        <v>90810</v>
+        <v>91076</v>
       </c>
       <c r="I310">
-        <v>5414</v>
+        <v>5190</v>
       </c>
     </row>
     <row r="311">
@@ -8081,10 +8081,10 @@
         <v>2918</v>
       </c>
       <c r="H311">
-        <v>37385</v>
+        <v>37117</v>
       </c>
       <c r="I311">
-        <v>1401</v>
+        <v>1395</v>
       </c>
     </row>
     <row r="312">
@@ -8139,10 +8139,10 @@
         <v>3102</v>
       </c>
       <c r="H313">
-        <v>72891</v>
+        <v>72960</v>
       </c>
       <c r="I313">
-        <v>3546</v>
+        <v>3553</v>
       </c>
     </row>
     <row r="314">
@@ -8168,7 +8168,7 @@
         <v>3163</v>
       </c>
       <c r="H314">
-        <v>65070</v>
+        <v>65084</v>
       </c>
       <c r="I314">
         <v>3346</v>
@@ -8197,10 +8197,10 @@
         <v>3260</v>
       </c>
       <c r="H315">
-        <v>66051</v>
+        <v>66203</v>
       </c>
       <c r="I315">
-        <v>3010</v>
+        <v>3011</v>
       </c>
     </row>
     <row r="316">
@@ -8226,7 +8226,7 @@
         <v>3362</v>
       </c>
       <c r="H316">
-        <v>49040</v>
+        <v>49037</v>
       </c>
       <c r="I316">
         <v>2278</v>
@@ -8255,7 +8255,7 @@
         <v>3417</v>
       </c>
       <c r="H317">
-        <v>61022</v>
+        <v>61174</v>
       </c>
       <c r="I317">
         <v>2124</v>
@@ -8284,10 +8284,10 @@
         <v>3474</v>
       </c>
       <c r="H318">
-        <v>24692</v>
+        <v>25032</v>
       </c>
       <c r="I318">
-        <v>888</v>
+        <v>925</v>
       </c>
     </row>
     <row r="319">
@@ -8342,10 +8342,10 @@
         <v>3637</v>
       </c>
       <c r="H320">
-        <v>86035</v>
+        <v>86146</v>
       </c>
       <c r="I320">
-        <v>4194</v>
+        <v>3892</v>
       </c>
     </row>
     <row r="321">
@@ -8371,10 +8371,10 @@
         <v>3737</v>
       </c>
       <c r="H321">
-        <v>86604</v>
+        <v>88965</v>
       </c>
       <c r="I321">
-        <v>2686</v>
+        <v>2766</v>
       </c>
     </row>
     <row r="322">
@@ -8400,10 +8400,10 @@
         <v>3801</v>
       </c>
       <c r="H322">
-        <v>102224</v>
+        <v>104338</v>
       </c>
       <c r="I322">
-        <v>2255</v>
+        <v>2288</v>
       </c>
     </row>
     <row r="323">
@@ -8429,10 +8429,10 @@
         <v>3894</v>
       </c>
       <c r="H323">
-        <v>143426</v>
+        <v>147242</v>
       </c>
       <c r="I323">
-        <v>2235</v>
+        <v>2294</v>
       </c>
     </row>
     <row r="324">
@@ -8458,10 +8458,10 @@
         <v>3965</v>
       </c>
       <c r="H324">
-        <v>209823</v>
+        <v>221337</v>
       </c>
       <c r="I324">
-        <v>2458</v>
+        <v>2590</v>
       </c>
     </row>
     <row r="325">
@@ -8487,10 +8487,10 @@
         <v>4068</v>
       </c>
       <c r="H325">
-        <v>562488</v>
+        <v>593430</v>
       </c>
       <c r="I325">
-        <v>5346</v>
+        <v>5572</v>
       </c>
     </row>
     <row r="326">
@@ -8516,10 +8516,10 @@
         <v>4068</v>
       </c>
       <c r="H326">
-        <v>284768</v>
+        <v>326887</v>
       </c>
       <c r="I326">
-        <v>2322</v>
+        <v>2687</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated: st 27. 01. 2021
</commit_message>
<xml_diff>
--- a/OpenData_Slovakia_Covid_DailyStats.xlsx
+++ b/OpenData_Slovakia_Covid_DailyStats.xlsx
@@ -6573,7 +6573,7 @@
         <v>579</v>
       </c>
       <c r="H259">
-        <v>6104</v>
+        <v>6086</v>
       </c>
       <c r="I259">
         <v>419</v>
@@ -6979,10 +6979,10 @@
         <v>930</v>
       </c>
       <c r="H273">
-        <v>27150</v>
+        <v>27129</v>
       </c>
       <c r="I273">
-        <v>1367</v>
+        <v>1366</v>
       </c>
     </row>
     <row r="274">
@@ -7124,7 +7124,7 @@
         <v>1046</v>
       </c>
       <c r="H278">
-        <v>30001</v>
+        <v>30006</v>
       </c>
       <c r="I278">
         <v>2101</v>
@@ -7385,7 +7385,7 @@
         <v>1378</v>
       </c>
       <c r="H287">
-        <v>57619</v>
+        <v>57649</v>
       </c>
       <c r="I287">
         <v>3917</v>
@@ -7762,7 +7762,7 @@
         <v>2065</v>
       </c>
       <c r="H300">
-        <v>70476</v>
+        <v>70463</v>
       </c>
       <c r="I300">
         <v>6917</v>
@@ -7791,7 +7791,7 @@
         <v>2138</v>
       </c>
       <c r="H301">
-        <v>69571</v>
+        <v>69574</v>
       </c>
       <c r="I301">
         <v>5560</v>
@@ -7878,7 +7878,7 @@
         <v>2317</v>
       </c>
       <c r="H304">
-        <v>6506</v>
+        <v>6503</v>
       </c>
       <c r="I304">
         <v>476</v>
@@ -7936,7 +7936,7 @@
         <v>2603</v>
       </c>
       <c r="H306">
-        <v>70729</v>
+        <v>70737</v>
       </c>
       <c r="I306">
         <v>7182</v>
@@ -8139,7 +8139,7 @@
         <v>3102</v>
       </c>
       <c r="H313">
-        <v>72960</v>
+        <v>72991</v>
       </c>
       <c r="I313">
         <v>3553</v>
@@ -8255,10 +8255,10 @@
         <v>3417</v>
       </c>
       <c r="H317">
-        <v>61174</v>
+        <v>61554</v>
       </c>
       <c r="I317">
-        <v>2124</v>
+        <v>2143</v>
       </c>
     </row>
     <row r="318">
@@ -8284,10 +8284,10 @@
         <v>3474</v>
       </c>
       <c r="H318">
-        <v>25032</v>
+        <v>24652</v>
       </c>
       <c r="I318">
-        <v>925</v>
+        <v>906</v>
       </c>
     </row>
     <row r="319">
@@ -8313,10 +8313,10 @@
         <v>3526</v>
       </c>
       <c r="H319">
-        <v>40781</v>
+        <v>56096</v>
       </c>
       <c r="I319">
-        <v>783</v>
+        <v>1785</v>
       </c>
     </row>
     <row r="320">
@@ -8342,10 +8342,10 @@
         <v>3637</v>
       </c>
       <c r="H320">
-        <v>86146</v>
+        <v>86149</v>
       </c>
       <c r="I320">
-        <v>3892</v>
+        <v>3893</v>
       </c>
     </row>
     <row r="321">
@@ -8371,10 +8371,10 @@
         <v>3737</v>
       </c>
       <c r="H321">
-        <v>88965</v>
+        <v>90179</v>
       </c>
       <c r="I321">
-        <v>2766</v>
+        <v>2796</v>
       </c>
     </row>
     <row r="322">
@@ -8400,10 +8400,10 @@
         <v>3801</v>
       </c>
       <c r="H322">
-        <v>104338</v>
+        <v>104385</v>
       </c>
       <c r="I322">
-        <v>2288</v>
+        <v>2287</v>
       </c>
     </row>
     <row r="323">
@@ -8429,10 +8429,10 @@
         <v>3894</v>
       </c>
       <c r="H323">
-        <v>147242</v>
+        <v>148033</v>
       </c>
       <c r="I323">
-        <v>2294</v>
+        <v>2317</v>
       </c>
     </row>
     <row r="324">
@@ -8458,10 +8458,10 @@
         <v>3965</v>
       </c>
       <c r="H324">
-        <v>221337</v>
+        <v>230592</v>
       </c>
       <c r="I324">
-        <v>2590</v>
+        <v>2665</v>
       </c>
     </row>
     <row r="325">
@@ -8487,10 +8487,10 @@
         <v>4068</v>
       </c>
       <c r="H325">
-        <v>593430</v>
+        <v>664115</v>
       </c>
       <c r="I325">
-        <v>5572</v>
+        <v>5455</v>
       </c>
     </row>
     <row r="326">
@@ -8516,10 +8516,10 @@
         <v>4068</v>
       </c>
       <c r="H326">
-        <v>326887</v>
+        <v>391033</v>
       </c>
       <c r="I326">
-        <v>2687</v>
+        <v>3424</v>
       </c>
     </row>
     <row r="327">
@@ -8545,10 +8545,10 @@
         <v>4260</v>
       </c>
       <c r="H327">
-        <v>244187</v>
+        <v>261513</v>
       </c>
       <c r="I327">
-        <v>3571</v>
+        <v>3782</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated: št 28. 01. 2021
</commit_message>
<xml_diff>
--- a/OpenData_Slovakia_Covid_DailyStats.xlsx
+++ b/OpenData_Slovakia_Covid_DailyStats.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I328"/>
+  <dimension ref="A1:I329"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -6921,10 +6921,10 @@
         <v>868</v>
       </c>
       <c r="H271">
-        <v>42584</v>
+        <v>42644</v>
       </c>
       <c r="I271">
-        <v>1620</v>
+        <v>1624</v>
       </c>
     </row>
     <row r="272">
@@ -6950,7 +6950,7 @@
         <v>898</v>
       </c>
       <c r="H272">
-        <v>30999</v>
+        <v>31038</v>
       </c>
       <c r="I272">
         <v>1666</v>
@@ -6979,10 +6979,10 @@
         <v>930</v>
       </c>
       <c r="H273">
-        <v>27129</v>
+        <v>27170</v>
       </c>
       <c r="I273">
-        <v>1366</v>
+        <v>1367</v>
       </c>
     </row>
     <row r="274">
@@ -7008,10 +7008,10 @@
         <v>957</v>
       </c>
       <c r="H274">
-        <v>28390</v>
+        <v>28505</v>
       </c>
       <c r="I274">
-        <v>1348</v>
+        <v>1349</v>
       </c>
     </row>
     <row r="275">
@@ -7037,10 +7037,10 @@
         <v>981</v>
       </c>
       <c r="H275">
-        <v>28741</v>
+        <v>28935</v>
       </c>
       <c r="I275">
-        <v>1239</v>
+        <v>1243</v>
       </c>
     </row>
     <row r="276">
@@ -7124,10 +7124,10 @@
         <v>1046</v>
       </c>
       <c r="H278">
-        <v>30006</v>
+        <v>30137</v>
       </c>
       <c r="I278">
-        <v>2101</v>
+        <v>2108</v>
       </c>
     </row>
     <row r="279">
@@ -7153,7 +7153,7 @@
         <v>1084</v>
       </c>
       <c r="H279">
-        <v>43382</v>
+        <v>43499</v>
       </c>
       <c r="I279">
         <v>3143</v>
@@ -7182,10 +7182,10 @@
         <v>1104</v>
       </c>
       <c r="H280">
-        <v>35570</v>
+        <v>35723</v>
       </c>
       <c r="I280">
-        <v>2405</v>
+        <v>2409</v>
       </c>
     </row>
     <row r="281">
@@ -7211,10 +7211,10 @@
         <v>1122</v>
       </c>
       <c r="H281">
-        <v>45201</v>
+        <v>45351</v>
       </c>
       <c r="I281">
-        <v>3255</v>
+        <v>3257</v>
       </c>
     </row>
     <row r="282">
@@ -7240,10 +7240,10 @@
         <v>1148</v>
       </c>
       <c r="H282">
-        <v>46781</v>
+        <v>46962</v>
       </c>
       <c r="I282">
-        <v>2857</v>
+        <v>2862</v>
       </c>
     </row>
     <row r="283">
@@ -7327,10 +7327,10 @@
         <v>1251</v>
       </c>
       <c r="H285">
-        <v>40884</v>
+        <v>41051</v>
       </c>
       <c r="I285">
-        <v>3432</v>
+        <v>3446</v>
       </c>
     </row>
     <row r="286">
@@ -7356,10 +7356,10 @@
         <v>1309</v>
       </c>
       <c r="H286">
-        <v>54196</v>
+        <v>54367</v>
       </c>
       <c r="I286">
-        <v>4250</v>
+        <v>4261</v>
       </c>
     </row>
     <row r="287">
@@ -7385,10 +7385,10 @@
         <v>1378</v>
       </c>
       <c r="H287">
-        <v>57649</v>
+        <v>57813</v>
       </c>
       <c r="I287">
-        <v>3917</v>
+        <v>3927</v>
       </c>
     </row>
     <row r="288">
@@ -7414,10 +7414,10 @@
         <v>1440</v>
       </c>
       <c r="H288">
-        <v>56086</v>
+        <v>56278</v>
       </c>
       <c r="I288">
-        <v>3959</v>
+        <v>3961</v>
       </c>
     </row>
     <row r="289">
@@ -7443,10 +7443,10 @@
         <v>1510</v>
       </c>
       <c r="H289">
-        <v>64395</v>
+        <v>64611</v>
       </c>
       <c r="I289">
-        <v>3699</v>
+        <v>3707</v>
       </c>
     </row>
     <row r="290">
@@ -7530,10 +7530,10 @@
         <v>1618</v>
       </c>
       <c r="H292">
-        <v>81241</v>
+        <v>81543</v>
       </c>
       <c r="I292">
-        <v>7191</v>
+        <v>7210</v>
       </c>
     </row>
     <row r="293">
@@ -7559,10 +7559,10 @@
         <v>1686</v>
       </c>
       <c r="H293">
-        <v>81666</v>
+        <v>81994</v>
       </c>
       <c r="I293">
-        <v>5794</v>
+        <v>5800</v>
       </c>
     </row>
     <row r="294">
@@ -7588,10 +7588,10 @@
         <v>1732</v>
       </c>
       <c r="H294">
-        <v>90790</v>
+        <v>91081</v>
       </c>
       <c r="I294">
-        <v>5028</v>
+        <v>5044</v>
       </c>
     </row>
     <row r="295">
@@ -7733,10 +7733,10 @@
         <v>1983</v>
       </c>
       <c r="H299">
-        <v>64055</v>
+        <v>64312</v>
       </c>
       <c r="I299">
-        <v>6713</v>
+        <v>6731</v>
       </c>
     </row>
     <row r="300">
@@ -7762,10 +7762,10 @@
         <v>2065</v>
       </c>
       <c r="H300">
-        <v>70463</v>
+        <v>70686</v>
       </c>
       <c r="I300">
-        <v>6917</v>
+        <v>6929</v>
       </c>
     </row>
     <row r="301">
@@ -7791,10 +7791,10 @@
         <v>2138</v>
       </c>
       <c r="H301">
-        <v>69574</v>
+        <v>69831</v>
       </c>
       <c r="I301">
-        <v>5560</v>
+        <v>5566</v>
       </c>
     </row>
     <row r="302">
@@ -7820,7 +7820,7 @@
         <v>2250</v>
       </c>
       <c r="H302">
-        <v>72555</v>
+        <v>72786</v>
       </c>
       <c r="I302">
         <v>5284</v>
@@ -7936,10 +7936,10 @@
         <v>2603</v>
       </c>
       <c r="H306">
-        <v>70737</v>
+        <v>70962</v>
       </c>
       <c r="I306">
-        <v>7182</v>
+        <v>7186</v>
       </c>
     </row>
     <row r="307">
@@ -7965,10 +7965,10 @@
         <v>2657</v>
       </c>
       <c r="H307">
-        <v>73347</v>
+        <v>73503</v>
       </c>
       <c r="I307">
-        <v>6323</v>
+        <v>6330</v>
       </c>
     </row>
     <row r="308">
@@ -8023,10 +8023,10 @@
         <v>2788</v>
       </c>
       <c r="H309">
-        <v>57315</v>
+        <v>57439</v>
       </c>
       <c r="I309">
-        <v>3962</v>
+        <v>3971</v>
       </c>
     </row>
     <row r="310">
@@ -8052,10 +8052,10 @@
         <v>2836</v>
       </c>
       <c r="H310">
-        <v>91076</v>
+        <v>91188</v>
       </c>
       <c r="I310">
-        <v>5190</v>
+        <v>5198</v>
       </c>
     </row>
     <row r="311">
@@ -8139,10 +8139,10 @@
         <v>3102</v>
       </c>
       <c r="H313">
-        <v>72991</v>
+        <v>73159</v>
       </c>
       <c r="I313">
-        <v>3553</v>
+        <v>3560</v>
       </c>
     </row>
     <row r="314">
@@ -8168,10 +8168,10 @@
         <v>3163</v>
       </c>
       <c r="H314">
-        <v>65084</v>
+        <v>65283</v>
       </c>
       <c r="I314">
-        <v>3346</v>
+        <v>3362</v>
       </c>
     </row>
     <row r="315">
@@ -8197,10 +8197,10 @@
         <v>3260</v>
       </c>
       <c r="H315">
-        <v>66203</v>
+        <v>66489</v>
       </c>
       <c r="I315">
-        <v>3011</v>
+        <v>3018</v>
       </c>
     </row>
     <row r="316">
@@ -8226,10 +8226,10 @@
         <v>3362</v>
       </c>
       <c r="H316">
-        <v>49037</v>
+        <v>49147</v>
       </c>
       <c r="I316">
-        <v>2278</v>
+        <v>2281</v>
       </c>
     </row>
     <row r="317">
@@ -8255,10 +8255,10 @@
         <v>3417</v>
       </c>
       <c r="H317">
-        <v>61554</v>
+        <v>61819</v>
       </c>
       <c r="I317">
-        <v>2143</v>
+        <v>2153</v>
       </c>
     </row>
     <row r="318">
@@ -8342,10 +8342,10 @@
         <v>3637</v>
       </c>
       <c r="H320">
-        <v>86149</v>
+        <v>86520</v>
       </c>
       <c r="I320">
-        <v>3893</v>
+        <v>3912</v>
       </c>
     </row>
     <row r="321">
@@ -8371,10 +8371,10 @@
         <v>3737</v>
       </c>
       <c r="H321">
-        <v>90179</v>
+        <v>90442</v>
       </c>
       <c r="I321">
-        <v>2796</v>
+        <v>2799</v>
       </c>
     </row>
     <row r="322">
@@ -8400,10 +8400,10 @@
         <v>3801</v>
       </c>
       <c r="H322">
-        <v>104385</v>
+        <v>104742</v>
       </c>
       <c r="I322">
-        <v>2287</v>
+        <v>2286</v>
       </c>
     </row>
     <row r="323">
@@ -8429,10 +8429,10 @@
         <v>3894</v>
       </c>
       <c r="H323">
-        <v>148033</v>
+        <v>149944</v>
       </c>
       <c r="I323">
-        <v>2317</v>
+        <v>2328</v>
       </c>
     </row>
     <row r="324">
@@ -8458,10 +8458,10 @@
         <v>3965</v>
       </c>
       <c r="H324">
-        <v>230592</v>
+        <v>231451</v>
       </c>
       <c r="I324">
-        <v>2665</v>
+        <v>2669</v>
       </c>
     </row>
     <row r="325">
@@ -8487,10 +8487,10 @@
         <v>4068</v>
       </c>
       <c r="H325">
-        <v>664115</v>
+        <v>667595</v>
       </c>
       <c r="I325">
-        <v>5455</v>
+        <v>5477</v>
       </c>
     </row>
     <row r="326">
@@ -8516,10 +8516,10 @@
         <v>4068</v>
       </c>
       <c r="H326">
-        <v>391033</v>
+        <v>402981</v>
       </c>
       <c r="I326">
-        <v>3424</v>
+        <v>3517</v>
       </c>
     </row>
     <row r="327">
@@ -8545,10 +8545,10 @@
         <v>4260</v>
       </c>
       <c r="H327">
-        <v>261513</v>
+        <v>253197</v>
       </c>
       <c r="I327">
-        <v>3782</v>
+        <v>3772</v>
       </c>
     </row>
     <row r="328">
@@ -8574,10 +8574,39 @@
         <v>4361</v>
       </c>
       <c r="H328">
-        <v>177450</v>
+        <v>188092</v>
       </c>
       <c r="I328">
-        <v>2599</v>
+        <v>2734</v>
+      </c>
+    </row>
+    <row r="329">
+      <c r="A329" s="2">
+        <v>44223</v>
+      </c>
+      <c r="B329">
+        <v>243427</v>
+      </c>
+      <c r="C329">
+        <v>205247</v>
+      </c>
+      <c r="D329">
+        <v>33769</v>
+      </c>
+      <c r="E329">
+        <v>9811</v>
+      </c>
+      <c r="F329">
+        <v>2035</v>
+      </c>
+      <c r="G329">
+        <v>4411</v>
+      </c>
+      <c r="H329">
+        <v>78633</v>
+      </c>
+      <c r="I329">
+        <v>1779</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated: pi 29. 01. 2021
</commit_message>
<xml_diff>
--- a/OpenData_Slovakia_Covid_DailyStats.xlsx
+++ b/OpenData_Slovakia_Covid_DailyStats.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I329"/>
+  <dimension ref="A1:I330"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -6950,10 +6950,10 @@
         <v>898</v>
       </c>
       <c r="H272">
-        <v>31038</v>
+        <v>30918</v>
       </c>
       <c r="I272">
-        <v>1666</v>
+        <v>1662</v>
       </c>
     </row>
     <row r="273">
@@ -7008,10 +7008,10 @@
         <v>957</v>
       </c>
       <c r="H274">
-        <v>28505</v>
+        <v>28351</v>
       </c>
       <c r="I274">
-        <v>1349</v>
+        <v>1348</v>
       </c>
     </row>
     <row r="275">
@@ -7037,10 +7037,10 @@
         <v>981</v>
       </c>
       <c r="H275">
-        <v>28935</v>
+        <v>28741</v>
       </c>
       <c r="I275">
-        <v>1243</v>
+        <v>1239</v>
       </c>
     </row>
     <row r="276">
@@ -7124,10 +7124,10 @@
         <v>1046</v>
       </c>
       <c r="H278">
-        <v>30137</v>
+        <v>29812</v>
       </c>
       <c r="I278">
-        <v>2108</v>
+        <v>2097</v>
       </c>
     </row>
     <row r="279">
@@ -7153,7 +7153,7 @@
         <v>1084</v>
       </c>
       <c r="H279">
-        <v>43499</v>
+        <v>43382</v>
       </c>
       <c r="I279">
         <v>3143</v>
@@ -7182,10 +7182,10 @@
         <v>1104</v>
       </c>
       <c r="H280">
-        <v>35723</v>
+        <v>35570</v>
       </c>
       <c r="I280">
-        <v>2409</v>
+        <v>2405</v>
       </c>
     </row>
     <row r="281">
@@ -7240,10 +7240,10 @@
         <v>1148</v>
       </c>
       <c r="H282">
-        <v>46962</v>
+        <v>46812</v>
       </c>
       <c r="I282">
-        <v>2862</v>
+        <v>2860</v>
       </c>
     </row>
     <row r="283">
@@ -7327,10 +7327,10 @@
         <v>1251</v>
       </c>
       <c r="H285">
-        <v>41051</v>
+        <v>40884</v>
       </c>
       <c r="I285">
-        <v>3446</v>
+        <v>3432</v>
       </c>
     </row>
     <row r="286">
@@ -7356,10 +7356,10 @@
         <v>1309</v>
       </c>
       <c r="H286">
-        <v>54367</v>
+        <v>54196</v>
       </c>
       <c r="I286">
-        <v>4261</v>
+        <v>4250</v>
       </c>
     </row>
     <row r="287">
@@ -7385,10 +7385,10 @@
         <v>1378</v>
       </c>
       <c r="H287">
-        <v>57813</v>
+        <v>57649</v>
       </c>
       <c r="I287">
-        <v>3927</v>
+        <v>3917</v>
       </c>
     </row>
     <row r="288">
@@ -7414,10 +7414,10 @@
         <v>1440</v>
       </c>
       <c r="H288">
-        <v>56278</v>
+        <v>56086</v>
       </c>
       <c r="I288">
-        <v>3961</v>
+        <v>3959</v>
       </c>
     </row>
     <row r="289">
@@ -7443,10 +7443,10 @@
         <v>1510</v>
       </c>
       <c r="H289">
-        <v>64611</v>
+        <v>64395</v>
       </c>
       <c r="I289">
-        <v>3707</v>
+        <v>3699</v>
       </c>
     </row>
     <row r="290">
@@ -7530,10 +7530,10 @@
         <v>1618</v>
       </c>
       <c r="H292">
-        <v>81543</v>
+        <v>81241</v>
       </c>
       <c r="I292">
-        <v>7210</v>
+        <v>7191</v>
       </c>
     </row>
     <row r="293">
@@ -7559,10 +7559,10 @@
         <v>1686</v>
       </c>
       <c r="H293">
-        <v>81994</v>
+        <v>81666</v>
       </c>
       <c r="I293">
-        <v>5800</v>
+        <v>5794</v>
       </c>
     </row>
     <row r="294">
@@ -7588,10 +7588,10 @@
         <v>1732</v>
       </c>
       <c r="H294">
-        <v>91081</v>
+        <v>90790</v>
       </c>
       <c r="I294">
-        <v>5044</v>
+        <v>5025</v>
       </c>
     </row>
     <row r="295">
@@ -7733,10 +7733,10 @@
         <v>1983</v>
       </c>
       <c r="H299">
-        <v>64312</v>
+        <v>64055</v>
       </c>
       <c r="I299">
-        <v>6731</v>
+        <v>6724</v>
       </c>
     </row>
     <row r="300">
@@ -7762,10 +7762,10 @@
         <v>2065</v>
       </c>
       <c r="H300">
-        <v>70686</v>
+        <v>70463</v>
       </c>
       <c r="I300">
-        <v>6929</v>
+        <v>6917</v>
       </c>
     </row>
     <row r="301">
@@ -7791,10 +7791,10 @@
         <v>2138</v>
       </c>
       <c r="H301">
-        <v>69831</v>
+        <v>69574</v>
       </c>
       <c r="I301">
-        <v>5566</v>
+        <v>5560</v>
       </c>
     </row>
     <row r="302">
@@ -7820,10 +7820,10 @@
         <v>2250</v>
       </c>
       <c r="H302">
-        <v>72786</v>
+        <v>72555</v>
       </c>
       <c r="I302">
-        <v>5284</v>
+        <v>5272</v>
       </c>
     </row>
     <row r="303">
@@ -7936,10 +7936,10 @@
         <v>2603</v>
       </c>
       <c r="H306">
-        <v>70962</v>
+        <v>70746</v>
       </c>
       <c r="I306">
-        <v>7186</v>
+        <v>7172</v>
       </c>
     </row>
     <row r="307">
@@ -7965,10 +7965,10 @@
         <v>2657</v>
       </c>
       <c r="H307">
-        <v>73503</v>
+        <v>73347</v>
       </c>
       <c r="I307">
-        <v>6330</v>
+        <v>6323</v>
       </c>
     </row>
     <row r="308">
@@ -8023,10 +8023,10 @@
         <v>2788</v>
       </c>
       <c r="H309">
-        <v>57439</v>
+        <v>57315</v>
       </c>
       <c r="I309">
-        <v>3971</v>
+        <v>3962</v>
       </c>
     </row>
     <row r="310">
@@ -8052,10 +8052,10 @@
         <v>2836</v>
       </c>
       <c r="H310">
-        <v>91188</v>
+        <v>90964</v>
       </c>
       <c r="I310">
-        <v>5198</v>
+        <v>5190</v>
       </c>
     </row>
     <row r="311">
@@ -8139,10 +8139,10 @@
         <v>3102</v>
       </c>
       <c r="H313">
-        <v>73159</v>
+        <v>72991</v>
       </c>
       <c r="I313">
-        <v>3560</v>
+        <v>3552</v>
       </c>
     </row>
     <row r="314">
@@ -8168,10 +8168,10 @@
         <v>3163</v>
       </c>
       <c r="H314">
-        <v>65283</v>
+        <v>65084</v>
       </c>
       <c r="I314">
-        <v>3362</v>
+        <v>3346</v>
       </c>
     </row>
     <row r="315">
@@ -8197,10 +8197,10 @@
         <v>3260</v>
       </c>
       <c r="H315">
-        <v>66489</v>
+        <v>66364</v>
       </c>
       <c r="I315">
-        <v>3018</v>
+        <v>3012</v>
       </c>
     </row>
     <row r="316">
@@ -8255,10 +8255,10 @@
         <v>3417</v>
       </c>
       <c r="H317">
-        <v>61819</v>
+        <v>61554</v>
       </c>
       <c r="I317">
-        <v>2153</v>
+        <v>2142</v>
       </c>
     </row>
     <row r="318">
@@ -8342,10 +8342,10 @@
         <v>3637</v>
       </c>
       <c r="H320">
-        <v>86520</v>
+        <v>86293</v>
       </c>
       <c r="I320">
-        <v>3912</v>
+        <v>3895</v>
       </c>
     </row>
     <row r="321">
@@ -8371,10 +8371,10 @@
         <v>3737</v>
       </c>
       <c r="H321">
-        <v>90442</v>
+        <v>90180</v>
       </c>
       <c r="I321">
-        <v>2799</v>
+        <v>2796</v>
       </c>
     </row>
     <row r="322">
@@ -8400,7 +8400,7 @@
         <v>3801</v>
       </c>
       <c r="H322">
-        <v>104742</v>
+        <v>104457</v>
       </c>
       <c r="I322">
         <v>2286</v>
@@ -8429,7 +8429,7 @@
         <v>3894</v>
       </c>
       <c r="H323">
-        <v>149944</v>
+        <v>150035</v>
       </c>
       <c r="I323">
         <v>2328</v>
@@ -8458,10 +8458,10 @@
         <v>3965</v>
       </c>
       <c r="H324">
-        <v>231451</v>
+        <v>231685</v>
       </c>
       <c r="I324">
-        <v>2669</v>
+        <v>2667</v>
       </c>
     </row>
     <row r="325">
@@ -8487,10 +8487,10 @@
         <v>4068</v>
       </c>
       <c r="H325">
-        <v>667595</v>
+        <v>673247</v>
       </c>
       <c r="I325">
-        <v>5477</v>
+        <v>5517</v>
       </c>
     </row>
     <row r="326">
@@ -8516,10 +8516,10 @@
         <v>4068</v>
       </c>
       <c r="H326">
-        <v>402981</v>
+        <v>404675</v>
       </c>
       <c r="I326">
-        <v>3517</v>
+        <v>3529</v>
       </c>
     </row>
     <row r="327">
@@ -8545,10 +8545,10 @@
         <v>4260</v>
       </c>
       <c r="H327">
-        <v>253197</v>
+        <v>253652</v>
       </c>
       <c r="I327">
-        <v>3772</v>
+        <v>3774</v>
       </c>
     </row>
     <row r="328">
@@ -8574,10 +8574,10 @@
         <v>4361</v>
       </c>
       <c r="H328">
-        <v>188092</v>
+        <v>189102</v>
       </c>
       <c r="I328">
-        <v>2734</v>
+        <v>2751</v>
       </c>
     </row>
     <row r="329">
@@ -8603,10 +8603,39 @@
         <v>4411</v>
       </c>
       <c r="H329">
-        <v>78633</v>
+        <v>82357</v>
       </c>
       <c r="I329">
-        <v>1779</v>
+        <v>1845</v>
+      </c>
+    </row>
+    <row r="330">
+      <c r="A330" s="2">
+        <v>44224</v>
+      </c>
+      <c r="B330">
+        <v>246008</v>
+      </c>
+      <c r="C330">
+        <v>208406</v>
+      </c>
+      <c r="D330">
+        <v>33107</v>
+      </c>
+      <c r="E330">
+        <v>11293</v>
+      </c>
+      <c r="F330">
+        <v>2581</v>
+      </c>
+      <c r="G330">
+        <v>4495</v>
+      </c>
+      <c r="H330">
+        <v>66287</v>
+      </c>
+      <c r="I330">
+        <v>5098</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated: po 01. 02. 2021
</commit_message>
<xml_diff>
--- a/OpenData_Slovakia_Covid_DailyStats.xlsx
+++ b/OpenData_Slovakia_Covid_DailyStats.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I330"/>
+  <dimension ref="A1:I333"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -6834,10 +6834,10 @@
         <v>798</v>
       </c>
       <c r="H268">
-        <v>14021</v>
+        <v>13814</v>
       </c>
       <c r="I268">
-        <v>687</v>
+        <v>666</v>
       </c>
     </row>
     <row r="269">
@@ -6921,10 +6921,10 @@
         <v>868</v>
       </c>
       <c r="H271">
-        <v>42644</v>
+        <v>42725</v>
       </c>
       <c r="I271">
-        <v>1624</v>
+        <v>1655</v>
       </c>
     </row>
     <row r="272">
@@ -6950,10 +6950,10 @@
         <v>898</v>
       </c>
       <c r="H272">
-        <v>30918</v>
+        <v>30441</v>
       </c>
       <c r="I272">
-        <v>1662</v>
+        <v>1638</v>
       </c>
     </row>
     <row r="273">
@@ -6979,10 +6979,10 @@
         <v>930</v>
       </c>
       <c r="H273">
-        <v>27170</v>
+        <v>26934</v>
       </c>
       <c r="I273">
-        <v>1367</v>
+        <v>1343</v>
       </c>
     </row>
     <row r="274">
@@ -7008,10 +7008,10 @@
         <v>957</v>
       </c>
       <c r="H274">
-        <v>28351</v>
+        <v>28546</v>
       </c>
       <c r="I274">
-        <v>1348</v>
+        <v>1325</v>
       </c>
     </row>
     <row r="275">
@@ -7037,10 +7037,10 @@
         <v>981</v>
       </c>
       <c r="H275">
-        <v>28741</v>
+        <v>29139</v>
       </c>
       <c r="I275">
-        <v>1239</v>
+        <v>1251</v>
       </c>
     </row>
     <row r="276">
@@ -7066,10 +7066,10 @@
         <v>996</v>
       </c>
       <c r="H276">
-        <v>13295</v>
+        <v>11741</v>
       </c>
       <c r="I276">
-        <v>454</v>
+        <v>418</v>
       </c>
     </row>
     <row r="277">
@@ -7124,10 +7124,10 @@
         <v>1046</v>
       </c>
       <c r="H278">
-        <v>29812</v>
+        <v>30008</v>
       </c>
       <c r="I278">
-        <v>2097</v>
+        <v>2128</v>
       </c>
     </row>
     <row r="279">
@@ -7153,10 +7153,10 @@
         <v>1084</v>
       </c>
       <c r="H279">
-        <v>43382</v>
+        <v>42946</v>
       </c>
       <c r="I279">
-        <v>3143</v>
+        <v>3100</v>
       </c>
     </row>
     <row r="280">
@@ -7182,10 +7182,10 @@
         <v>1104</v>
       </c>
       <c r="H280">
-        <v>35570</v>
+        <v>35112</v>
       </c>
       <c r="I280">
-        <v>2405</v>
+        <v>2351</v>
       </c>
     </row>
     <row r="281">
@@ -7211,10 +7211,10 @@
         <v>1122</v>
       </c>
       <c r="H281">
-        <v>45351</v>
+        <v>45427</v>
       </c>
       <c r="I281">
-        <v>3257</v>
+        <v>3286</v>
       </c>
     </row>
     <row r="282">
@@ -7240,10 +7240,10 @@
         <v>1148</v>
       </c>
       <c r="H282">
-        <v>46812</v>
+        <v>47241</v>
       </c>
       <c r="I282">
-        <v>2860</v>
+        <v>2845</v>
       </c>
     </row>
     <row r="283">
@@ -7269,10 +7269,10 @@
         <v>1175</v>
       </c>
       <c r="H283">
-        <v>17556</v>
+        <v>16913</v>
       </c>
       <c r="I283">
-        <v>1036</v>
+        <v>1001</v>
       </c>
     </row>
     <row r="284">
@@ -7327,10 +7327,10 @@
         <v>1251</v>
       </c>
       <c r="H285">
-        <v>40884</v>
+        <v>41494</v>
       </c>
       <c r="I285">
-        <v>3432</v>
+        <v>3462</v>
       </c>
     </row>
     <row r="286">
@@ -7356,10 +7356,10 @@
         <v>1309</v>
       </c>
       <c r="H286">
-        <v>54196</v>
+        <v>54662</v>
       </c>
       <c r="I286">
-        <v>4250</v>
+        <v>4267</v>
       </c>
     </row>
     <row r="287">
@@ -7385,10 +7385,10 @@
         <v>1378</v>
       </c>
       <c r="H287">
-        <v>57649</v>
+        <v>57746</v>
       </c>
       <c r="I287">
-        <v>3917</v>
+        <v>3920</v>
       </c>
     </row>
     <row r="288">
@@ -7414,10 +7414,10 @@
         <v>1440</v>
       </c>
       <c r="H288">
-        <v>56086</v>
+        <v>57099</v>
       </c>
       <c r="I288">
-        <v>3959</v>
+        <v>4000</v>
       </c>
     </row>
     <row r="289">
@@ -7443,10 +7443,10 @@
         <v>1510</v>
       </c>
       <c r="H289">
-        <v>64395</v>
+        <v>63138</v>
       </c>
       <c r="I289">
-        <v>3699</v>
+        <v>3623</v>
       </c>
     </row>
     <row r="290">
@@ -7472,10 +7472,10 @@
         <v>1555</v>
       </c>
       <c r="H290">
-        <v>17876</v>
+        <v>17626</v>
       </c>
       <c r="I290">
-        <v>1489</v>
+        <v>1474</v>
       </c>
     </row>
     <row r="291">
@@ -7501,7 +7501,7 @@
         <v>1618</v>
       </c>
       <c r="H291">
-        <v>14831</v>
+        <v>14851</v>
       </c>
       <c r="I291">
         <v>483</v>
@@ -7530,10 +7530,10 @@
         <v>1618</v>
       </c>
       <c r="H292">
-        <v>81241</v>
+        <v>81769</v>
       </c>
       <c r="I292">
-        <v>7191</v>
+        <v>7255</v>
       </c>
     </row>
     <row r="293">
@@ -7559,10 +7559,10 @@
         <v>1686</v>
       </c>
       <c r="H293">
-        <v>81666</v>
+        <v>81657</v>
       </c>
       <c r="I293">
-        <v>5794</v>
+        <v>5745</v>
       </c>
     </row>
     <row r="294">
@@ -7588,10 +7588,10 @@
         <v>1732</v>
       </c>
       <c r="H294">
-        <v>90790</v>
+        <v>90992</v>
       </c>
       <c r="I294">
-        <v>5025</v>
+        <v>5040</v>
       </c>
     </row>
     <row r="295">
@@ -7617,10 +7617,10 @@
         <v>1732</v>
       </c>
       <c r="H295">
-        <v>19353</v>
+        <v>17958</v>
       </c>
       <c r="I295">
-        <v>1136</v>
+        <v>1056</v>
       </c>
     </row>
     <row r="296">
@@ -7733,10 +7733,10 @@
         <v>1983</v>
       </c>
       <c r="H299">
-        <v>64055</v>
+        <v>64544</v>
       </c>
       <c r="I299">
-        <v>6724</v>
+        <v>6802</v>
       </c>
     </row>
     <row r="300">
@@ -7762,10 +7762,10 @@
         <v>2065</v>
       </c>
       <c r="H300">
-        <v>70463</v>
+        <v>71397</v>
       </c>
       <c r="I300">
-        <v>6917</v>
+        <v>7028</v>
       </c>
     </row>
     <row r="301">
@@ -7791,10 +7791,10 @@
         <v>2138</v>
       </c>
       <c r="H301">
-        <v>69574</v>
+        <v>69695</v>
       </c>
       <c r="I301">
-        <v>5560</v>
+        <v>5555</v>
       </c>
     </row>
     <row r="302">
@@ -7820,10 +7820,10 @@
         <v>2250</v>
       </c>
       <c r="H302">
-        <v>72555</v>
+        <v>74110</v>
       </c>
       <c r="I302">
-        <v>5272</v>
+        <v>5364</v>
       </c>
     </row>
     <row r="303">
@@ -7849,10 +7849,10 @@
         <v>2250</v>
       </c>
       <c r="H303">
-        <v>11470</v>
+        <v>10165</v>
       </c>
       <c r="I303">
-        <v>753</v>
+        <v>665</v>
       </c>
     </row>
     <row r="304">
@@ -7878,7 +7878,7 @@
         <v>2317</v>
       </c>
       <c r="H304">
-        <v>6503</v>
+        <v>6511</v>
       </c>
       <c r="I304">
         <v>476</v>
@@ -7936,10 +7936,10 @@
         <v>2603</v>
       </c>
       <c r="H306">
-        <v>70746</v>
+        <v>71105</v>
       </c>
       <c r="I306">
-        <v>7172</v>
+        <v>7209</v>
       </c>
     </row>
     <row r="307">
@@ -7965,10 +7965,10 @@
         <v>2657</v>
       </c>
       <c r="H307">
-        <v>73347</v>
+        <v>74660</v>
       </c>
       <c r="I307">
-        <v>6323</v>
+        <v>6415</v>
       </c>
     </row>
     <row r="308">
@@ -7994,10 +7994,10 @@
         <v>2717</v>
       </c>
       <c r="H308">
-        <v>17044</v>
+        <v>15688</v>
       </c>
       <c r="I308">
-        <v>1425</v>
+        <v>1327</v>
       </c>
     </row>
     <row r="309">
@@ -8023,10 +8023,10 @@
         <v>2788</v>
       </c>
       <c r="H309">
-        <v>57315</v>
+        <v>58840</v>
       </c>
       <c r="I309">
-        <v>3962</v>
+        <v>4056</v>
       </c>
     </row>
     <row r="310">
@@ -8052,10 +8052,10 @@
         <v>2836</v>
       </c>
       <c r="H310">
-        <v>90964</v>
+        <v>91546</v>
       </c>
       <c r="I310">
-        <v>5190</v>
+        <v>5209</v>
       </c>
     </row>
     <row r="311">
@@ -8081,10 +8081,10 @@
         <v>2918</v>
       </c>
       <c r="H311">
-        <v>37117</v>
+        <v>36065</v>
       </c>
       <c r="I311">
-        <v>1395</v>
+        <v>1335</v>
       </c>
     </row>
     <row r="312">
@@ -8110,7 +8110,7 @@
         <v>3007</v>
       </c>
       <c r="H312">
-        <v>40569</v>
+        <v>40279</v>
       </c>
       <c r="I312">
         <v>1225</v>
@@ -8139,10 +8139,10 @@
         <v>3102</v>
       </c>
       <c r="H313">
-        <v>72991</v>
+        <v>73967</v>
       </c>
       <c r="I313">
-        <v>3552</v>
+        <v>3596</v>
       </c>
     </row>
     <row r="314">
@@ -8168,10 +8168,10 @@
         <v>3163</v>
       </c>
       <c r="H314">
-        <v>65084</v>
+        <v>64641</v>
       </c>
       <c r="I314">
-        <v>3346</v>
+        <v>3318</v>
       </c>
     </row>
     <row r="315">
@@ -8197,10 +8197,10 @@
         <v>3260</v>
       </c>
       <c r="H315">
-        <v>66364</v>
+        <v>65879</v>
       </c>
       <c r="I315">
-        <v>3012</v>
+        <v>2723</v>
       </c>
     </row>
     <row r="316">
@@ -8226,10 +8226,10 @@
         <v>3362</v>
       </c>
       <c r="H316">
-        <v>49147</v>
+        <v>48644</v>
       </c>
       <c r="I316">
-        <v>2281</v>
+        <v>2223</v>
       </c>
     </row>
     <row r="317">
@@ -8255,10 +8255,10 @@
         <v>3417</v>
       </c>
       <c r="H317">
-        <v>61554</v>
+        <v>61584</v>
       </c>
       <c r="I317">
-        <v>2142</v>
+        <v>2123</v>
       </c>
     </row>
     <row r="318">
@@ -8284,10 +8284,10 @@
         <v>3474</v>
       </c>
       <c r="H318">
-        <v>24652</v>
+        <v>23054</v>
       </c>
       <c r="I318">
-        <v>906</v>
+        <v>872</v>
       </c>
     </row>
     <row r="319">
@@ -8313,10 +8313,10 @@
         <v>3526</v>
       </c>
       <c r="H319">
-        <v>56096</v>
+        <v>56054</v>
       </c>
       <c r="I319">
-        <v>1785</v>
+        <v>1778</v>
       </c>
     </row>
     <row r="320">
@@ -8342,10 +8342,10 @@
         <v>3637</v>
       </c>
       <c r="H320">
-        <v>86293</v>
+        <v>87122</v>
       </c>
       <c r="I320">
-        <v>3895</v>
+        <v>3942</v>
       </c>
     </row>
     <row r="321">
@@ -8371,10 +8371,10 @@
         <v>3737</v>
       </c>
       <c r="H321">
-        <v>90180</v>
+        <v>90259</v>
       </c>
       <c r="I321">
-        <v>2796</v>
+        <v>2789</v>
       </c>
     </row>
     <row r="322">
@@ -8400,10 +8400,10 @@
         <v>3801</v>
       </c>
       <c r="H322">
-        <v>104457</v>
+        <v>105138</v>
       </c>
       <c r="I322">
-        <v>2286</v>
+        <v>2272</v>
       </c>
     </row>
     <row r="323">
@@ -8429,10 +8429,10 @@
         <v>3894</v>
       </c>
       <c r="H323">
-        <v>150035</v>
+        <v>147599</v>
       </c>
       <c r="I323">
-        <v>2328</v>
+        <v>2289</v>
       </c>
     </row>
     <row r="324">
@@ -8458,10 +8458,10 @@
         <v>3965</v>
       </c>
       <c r="H324">
-        <v>231685</v>
+        <v>230408</v>
       </c>
       <c r="I324">
-        <v>2667</v>
+        <v>2668</v>
       </c>
     </row>
     <row r="325">
@@ -8487,10 +8487,10 @@
         <v>4068</v>
       </c>
       <c r="H325">
-        <v>673247</v>
+        <v>684258</v>
       </c>
       <c r="I325">
-        <v>5517</v>
+        <v>5624</v>
       </c>
     </row>
     <row r="326">
@@ -8516,10 +8516,10 @@
         <v>4068</v>
       </c>
       <c r="H326">
-        <v>404675</v>
+        <v>408272</v>
       </c>
       <c r="I326">
-        <v>3529</v>
+        <v>3601</v>
       </c>
     </row>
     <row r="327">
@@ -8545,10 +8545,10 @@
         <v>4260</v>
       </c>
       <c r="H327">
-        <v>253652</v>
+        <v>257844</v>
       </c>
       <c r="I327">
-        <v>3774</v>
+        <v>3689</v>
       </c>
     </row>
     <row r="328">
@@ -8574,10 +8574,10 @@
         <v>4361</v>
       </c>
       <c r="H328">
-        <v>189102</v>
+        <v>187092</v>
       </c>
       <c r="I328">
-        <v>2751</v>
+        <v>2725</v>
       </c>
     </row>
     <row r="329">
@@ -8603,10 +8603,10 @@
         <v>4411</v>
       </c>
       <c r="H329">
-        <v>82357</v>
+        <v>82182</v>
       </c>
       <c r="I329">
-        <v>1845</v>
+        <v>1867</v>
       </c>
     </row>
     <row r="330">
@@ -8632,10 +8632,97 @@
         <v>4495</v>
       </c>
       <c r="H330">
-        <v>66287</v>
+        <v>68480</v>
       </c>
       <c r="I330">
-        <v>5098</v>
+        <v>1961</v>
+      </c>
+    </row>
+    <row r="331">
+      <c r="A331" s="2">
+        <v>44225</v>
+      </c>
+      <c r="B331">
+        <v>248190</v>
+      </c>
+      <c r="C331">
+        <v>212271</v>
+      </c>
+      <c r="D331">
+        <v>31354</v>
+      </c>
+      <c r="E331">
+        <v>11207</v>
+      </c>
+      <c r="F331">
+        <v>2182</v>
+      </c>
+      <c r="G331">
+        <v>4565</v>
+      </c>
+      <c r="H331">
+        <v>142646</v>
+      </c>
+      <c r="I331">
+        <v>2462</v>
+      </c>
+    </row>
+    <row r="332">
+      <c r="A332" s="2">
+        <v>44226</v>
+      </c>
+      <c r="B332">
+        <v>249913</v>
+      </c>
+      <c r="C332">
+        <v>216052</v>
+      </c>
+      <c r="D332">
+        <v>29219</v>
+      </c>
+      <c r="E332">
+        <v>8201</v>
+      </c>
+      <c r="F332">
+        <v>1723</v>
+      </c>
+      <c r="G332">
+        <v>4642</v>
+      </c>
+      <c r="H332">
+        <v>349642</v>
+      </c>
+      <c r="I332">
+        <v>4022</v>
+      </c>
+    </row>
+    <row r="333">
+      <c r="A333" s="2">
+        <v>44227</v>
+      </c>
+      <c r="B333">
+        <v>250357</v>
+      </c>
+      <c r="C333">
+        <v>218923</v>
+      </c>
+      <c r="D333">
+        <v>26723</v>
+      </c>
+      <c r="E333">
+        <v>2290</v>
+      </c>
+      <c r="F333">
+        <v>444</v>
+      </c>
+      <c r="G333">
+        <v>4711</v>
+      </c>
+      <c r="H333">
+        <v>204733</v>
+      </c>
+      <c r="I333">
+        <v>2127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated: ut 02. 02. 2021 (New file structure from 07.Feb.2021)
</commit_message>
<xml_diff>
--- a/OpenData_Slovakia_Covid_DailyStats.xlsx
+++ b/OpenData_Slovakia_Covid_DailyStats.xlsx
@@ -355,7 +355,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:I333"/>
+  <dimension ref="A1:I334"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -7588,10 +7588,10 @@
         <v>1732</v>
       </c>
       <c r="H294">
-        <v>90992</v>
+        <v>91360</v>
       </c>
       <c r="I294">
-        <v>5040</v>
+        <v>5061</v>
       </c>
     </row>
     <row r="295">
@@ -7762,10 +7762,10 @@
         <v>2065</v>
       </c>
       <c r="H300">
-        <v>71397</v>
+        <v>71698</v>
       </c>
       <c r="I300">
-        <v>7028</v>
+        <v>7031</v>
       </c>
     </row>
     <row r="301">
@@ -7820,10 +7820,10 @@
         <v>2250</v>
       </c>
       <c r="H302">
-        <v>74110</v>
+        <v>74114</v>
       </c>
       <c r="I302">
-        <v>5364</v>
+        <v>5365</v>
       </c>
     </row>
     <row r="303">
@@ -7849,10 +7849,10 @@
         <v>2250</v>
       </c>
       <c r="H303">
-        <v>10165</v>
+        <v>10423</v>
       </c>
       <c r="I303">
-        <v>665</v>
+        <v>666</v>
       </c>
     </row>
     <row r="304">
@@ -8081,10 +8081,10 @@
         <v>2918</v>
       </c>
       <c r="H311">
-        <v>36065</v>
+        <v>36069</v>
       </c>
       <c r="I311">
-        <v>1335</v>
+        <v>1337</v>
       </c>
     </row>
     <row r="312">
@@ -8110,7 +8110,7 @@
         <v>3007</v>
       </c>
       <c r="H312">
-        <v>40279</v>
+        <v>40269</v>
       </c>
       <c r="I312">
         <v>1225</v>
@@ -8255,10 +8255,10 @@
         <v>3417</v>
       </c>
       <c r="H317">
-        <v>61584</v>
+        <v>62528</v>
       </c>
       <c r="I317">
-        <v>2123</v>
+        <v>2131</v>
       </c>
     </row>
     <row r="318">
@@ -8313,10 +8313,10 @@
         <v>3526</v>
       </c>
       <c r="H319">
-        <v>56054</v>
+        <v>56550</v>
       </c>
       <c r="I319">
-        <v>1778</v>
+        <v>1787</v>
       </c>
     </row>
     <row r="320">
@@ -8342,10 +8342,10 @@
         <v>3637</v>
       </c>
       <c r="H320">
-        <v>87122</v>
+        <v>87570</v>
       </c>
       <c r="I320">
-        <v>3942</v>
+        <v>3964</v>
       </c>
     </row>
     <row r="321">
@@ -8371,10 +8371,10 @@
         <v>3737</v>
       </c>
       <c r="H321">
-        <v>90259</v>
+        <v>90401</v>
       </c>
       <c r="I321">
-        <v>2789</v>
+        <v>2788</v>
       </c>
     </row>
     <row r="322">
@@ -8400,10 +8400,10 @@
         <v>3801</v>
       </c>
       <c r="H322">
-        <v>105138</v>
+        <v>106230</v>
       </c>
       <c r="I322">
-        <v>2272</v>
+        <v>2280</v>
       </c>
     </row>
     <row r="323">
@@ -8429,10 +8429,10 @@
         <v>3894</v>
       </c>
       <c r="H323">
-        <v>147599</v>
+        <v>149018</v>
       </c>
       <c r="I323">
-        <v>2289</v>
+        <v>2307</v>
       </c>
     </row>
     <row r="324">
@@ -8458,10 +8458,10 @@
         <v>3965</v>
       </c>
       <c r="H324">
-        <v>230408</v>
+        <v>230440</v>
       </c>
       <c r="I324">
-        <v>2668</v>
+        <v>2636</v>
       </c>
     </row>
     <row r="325">
@@ -8487,10 +8487,10 @@
         <v>4068</v>
       </c>
       <c r="H325">
-        <v>684258</v>
+        <v>698532</v>
       </c>
       <c r="I325">
-        <v>5624</v>
+        <v>5756</v>
       </c>
     </row>
     <row r="326">
@@ -8516,10 +8516,10 @@
         <v>4068</v>
       </c>
       <c r="H326">
-        <v>408272</v>
+        <v>414294</v>
       </c>
       <c r="I326">
-        <v>3601</v>
+        <v>3641</v>
       </c>
     </row>
     <row r="327">
@@ -8545,10 +8545,10 @@
         <v>4260</v>
       </c>
       <c r="H327">
-        <v>257844</v>
+        <v>236946</v>
       </c>
       <c r="I327">
-        <v>3689</v>
+        <v>3536</v>
       </c>
     </row>
     <row r="328">
@@ -8574,10 +8574,10 @@
         <v>4361</v>
       </c>
       <c r="H328">
-        <v>187092</v>
+        <v>180211</v>
       </c>
       <c r="I328">
-        <v>2725</v>
+        <v>2634</v>
       </c>
     </row>
     <row r="329">
@@ -8603,7 +8603,7 @@
         <v>4411</v>
       </c>
       <c r="H329">
-        <v>82182</v>
+        <v>82184</v>
       </c>
       <c r="I329">
         <v>1867</v>
@@ -8632,10 +8632,10 @@
         <v>4495</v>
       </c>
       <c r="H330">
-        <v>68480</v>
+        <v>70555</v>
       </c>
       <c r="I330">
-        <v>1961</v>
+        <v>1970</v>
       </c>
     </row>
     <row r="331">
@@ -8661,10 +8661,10 @@
         <v>4565</v>
       </c>
       <c r="H331">
-        <v>142646</v>
+        <v>145637</v>
       </c>
       <c r="I331">
-        <v>2462</v>
+        <v>2490</v>
       </c>
     </row>
     <row r="332">
@@ -8690,10 +8690,10 @@
         <v>4642</v>
       </c>
       <c r="H332">
-        <v>349642</v>
+        <v>388839</v>
       </c>
       <c r="I332">
-        <v>4022</v>
+        <v>3758</v>
       </c>
     </row>
     <row r="333">
@@ -8719,10 +8719,39 @@
         <v>4711</v>
       </c>
       <c r="H333">
-        <v>204733</v>
+        <v>238056</v>
       </c>
       <c r="I333">
-        <v>2127</v>
+        <v>2533</v>
+      </c>
+    </row>
+    <row r="334">
+      <c r="A334" s="2">
+        <v>44228</v>
+      </c>
+      <c r="B334">
+        <v>252094</v>
+      </c>
+      <c r="C334">
+        <v>222642</v>
+      </c>
+      <c r="D334">
+        <v>24668</v>
+      </c>
+      <c r="E334">
+        <v>9504</v>
+      </c>
+      <c r="F334">
+        <v>1737</v>
+      </c>
+      <c r="G334">
+        <v>4784</v>
+      </c>
+      <c r="H334">
+        <v>184663</v>
+      </c>
+      <c r="I334">
+        <v>3242</v>
       </c>
     </row>
   </sheetData>

</xml_diff>